<commit_message>
create function to iterate every file
</commit_message>
<xml_diff>
--- a/Copypega.xlsx
+++ b/Copypega.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\AppData\Local\Programs\Python\Python312\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3003AA9D-0FFC-4A6E-B526-4A0A90D96D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9AD2A-7738-414A-B348-11E9A88FFB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="120">
   <si>
     <t>Ir al menu</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>Equipo de computo</t>
+  </si>
+  <si>
+    <t>Grupos de Estudio</t>
   </si>
 </sst>
 </file>
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E170"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:F171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,11 +993,11 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="9">
-        <v>647962.16</v>
+        <v>613000.13</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="9">
-        <v>609696.6</v>
+        <v>1385866.68</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="9"/>
@@ -1018,12 +1021,12 @@
         <v>7</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="20">
-        <v>0</v>
+      <c r="C13" s="14">
+        <v>150000</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="14">
-        <v>120000</v>
+        <v>169997.06</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1033,11 +1036,11 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="9">
-        <v>647962.16</v>
+        <v>763000.13</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="9">
-        <v>729696.6</v>
+        <v>1555863.74</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1064,8 +1067,8 @@
         <v>60</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="7">
-        <v>0</v>
+      <c r="C17" s="9">
+        <v>814142</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="7">
@@ -1083,7 +1086,7 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="9">
-        <v>439712.6</v>
+        <v>1238381.3799999999</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1121,11 +1124,11 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="9">
-        <v>45000</v>
+        <v>130485.56</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="7">
-        <v>0</v>
+      <c r="E21" s="9">
+        <v>135000.09</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1135,11 +1138,11 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="9">
-        <v>20000</v>
+        <v>44000</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="9">
-        <v>46000</v>
+        <v>10000</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -1163,11 +1166,11 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="9">
-        <v>65000</v>
+        <v>988627.56</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="9">
-        <v>485712.6</v>
+        <v>1383381.47</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -1202,12 +1205,12 @@
         <v>15</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="9">
-        <v>94064</v>
+      <c r="C28" s="7">
+        <v>0</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="9">
-        <v>31000</v>
+        <v>174352.33</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -1221,7 +1224,7 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="9">
-        <v>124999.87</v>
+        <v>53000</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -1272,12 +1275,12 @@
         <v>17</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="9">
-        <v>94064</v>
+      <c r="C33" s="7">
+        <v>0</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="9">
-        <v>155999.87</v>
+        <v>227352.33</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -1309,7 +1312,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="9">
-        <v>47810.7</v>
+        <v>55020.35</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -1351,7 +1354,7 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="9">
-        <v>47810.7</v>
+        <v>55020.35</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -1378,12 +1381,12 @@
         <v>46</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="9">
-        <v>339993.45</v>
+      <c r="C42" s="7">
+        <v>0</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="9">
-        <v>363991.3</v>
+      <c r="E42" s="7">
+        <v>0</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -1393,7 +1396,7 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="20">
-        <v>501.85</v>
+        <v>250.7</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="20">
@@ -1406,12 +1409,12 @@
         <v>48</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="9">
-        <v>340495.3</v>
+      <c r="C44" s="7">
+        <v>250.7</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="9">
-        <v>363991.3</v>
+      <c r="E44" s="7">
+        <v>0</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -1466,8 +1469,8 @@
         <v>62</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="7">
-        <v>0</v>
+      <c r="C49" s="9">
+        <v>75500</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="7">
@@ -1494,12 +1497,12 @@
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="7">
-        <v>0</v>
+      <c r="C51" s="9">
+        <v>11000</v>
       </c>
       <c r="D51" s="2"/>
-      <c r="E51" s="7">
-        <v>0</v>
+      <c r="E51" s="9">
+        <v>15999.99</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -1592,8 +1595,8 @@
         <v>76</v>
       </c>
       <c r="B58" s="2"/>
-      <c r="C58" s="14">
-        <v>20000</v>
+      <c r="C58" s="20">
+        <v>0</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="20">
@@ -1607,11 +1610,11 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="9">
-        <v>20000</v>
+        <v>86500</v>
       </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="7">
-        <v>0</v>
+      <c r="E59" s="9">
+        <v>15999.99</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -1629,11 +1632,11 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="15">
-        <v>1167521.46</v>
+        <v>1838378.39</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="15">
-        <v>1783211.07</v>
+        <v>3237617.88</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -1684,12 +1687,12 @@
         <v>23</v>
       </c>
       <c r="B66" s="2"/>
-      <c r="C66" s="7">
-        <v>0</v>
+      <c r="C66" s="9">
+        <v>350000</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="9">
-        <v>310000</v>
+        <v>223000</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -1698,8 +1701,8 @@
         <v>24</v>
       </c>
       <c r="B67" s="2"/>
-      <c r="C67" s="9">
-        <v>45000</v>
+      <c r="C67" s="7">
+        <v>0</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="9">
@@ -1730,8 +1733,8 @@
         <v>0</v>
       </c>
       <c r="D69" s="2"/>
-      <c r="E69" s="20">
-        <v>0</v>
+      <c r="E69" s="14">
+        <v>20000</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -1741,11 +1744,11 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="9">
-        <v>45000</v>
+        <v>350000</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="9">
-        <v>340000</v>
+        <v>273000</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -1762,12 +1765,12 @@
         <v>51</v>
       </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="9">
-        <v>21575</v>
+      <c r="C72" s="7">
+        <v>0</v>
       </c>
       <c r="D72" s="2"/>
-      <c r="E72" s="9">
-        <v>16115</v>
+      <c r="E72" s="7">
+        <v>0</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -1776,12 +1779,12 @@
         <v>27</v>
       </c>
       <c r="B73" s="2"/>
-      <c r="C73" s="9">
-        <v>16800</v>
+      <c r="C73" s="7">
+        <v>0</v>
       </c>
       <c r="D73" s="2"/>
-      <c r="E73" s="7">
-        <v>0</v>
+      <c r="E73" s="9">
+        <v>5000</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -1790,8 +1793,8 @@
         <v>52</v>
       </c>
       <c r="B74" s="2"/>
-      <c r="C74" s="20">
-        <v>0</v>
+      <c r="C74" s="14">
+        <v>99524.45</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="20">
@@ -1805,11 +1808,11 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="9">
-        <v>38375</v>
+        <v>99524.45</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="9">
-        <v>16115</v>
+        <v>5000</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -1849,11 +1852,11 @@
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="9">
-        <v>83375</v>
+        <v>449524.45</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="9">
-        <v>356115</v>
+        <v>278000</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -2001,7 +2004,7 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="9">
-        <v>58565</v>
+        <v>19000</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="7">
@@ -2014,12 +2017,12 @@
         <v>11</v>
       </c>
       <c r="B92" s="2"/>
-      <c r="C92" s="7">
-        <v>0</v>
+      <c r="C92" s="9">
+        <v>57891</v>
       </c>
       <c r="D92" s="2"/>
-      <c r="E92" s="7">
-        <v>0</v>
+      <c r="E92" s="9">
+        <v>75065</v>
       </c>
       <c r="F92" s="2"/>
     </row>
@@ -2028,12 +2031,12 @@
         <v>12</v>
       </c>
       <c r="B93" s="2"/>
-      <c r="C93" s="7">
-        <v>0</v>
+      <c r="C93" s="9">
+        <v>107832</v>
       </c>
       <c r="D93" s="2"/>
-      <c r="E93" s="9">
-        <v>29348</v>
+      <c r="E93" s="7">
+        <v>0</v>
       </c>
       <c r="F93" s="2"/>
     </row>
@@ -2042,8 +2045,8 @@
         <v>64</v>
       </c>
       <c r="B94" s="2"/>
-      <c r="C94" s="7">
-        <v>0</v>
+      <c r="C94" s="9">
+        <v>70985</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="7">
@@ -2079,46 +2082,50 @@
       </c>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" s="7">
+        <v>0</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="7">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="20">
-        <v>0</v>
-      </c>
-      <c r="D97" s="5"/>
-      <c r="E97" s="20">
-        <v>0</v>
-      </c>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
+      <c r="B98" s="2"/>
+      <c r="C98" s="20">
+        <v>0</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="20">
+        <v>0</v>
+      </c>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B98" s="2"/>
-      <c r="C98" s="9">
-        <v>58565</v>
-      </c>
-      <c r="D98" s="2"/>
-      <c r="E98" s="9">
-        <v>29348</v>
-      </c>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="2"/>
       <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
+      <c r="C99" s="9">
+        <v>255708</v>
+      </c>
       <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
+      <c r="E99" s="9">
+        <v>75065</v>
+      </c>
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -2126,50 +2133,46 @@
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B101" s="16"/>
-      <c r="C101" s="22">
-        <v>0</v>
-      </c>
-      <c r="D101" s="16"/>
-      <c r="E101" s="17">
-        <v>70540</v>
-      </c>
+      <c r="A101" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B102" s="16"/>
       <c r="C102" s="17">
-        <v>146912.94</v>
+        <v>77460</v>
       </c>
       <c r="D102" s="16"/>
       <c r="E102" s="17">
-        <v>22366.73</v>
+        <v>67625</v>
       </c>
       <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B103" s="16"/>
-      <c r="C103" s="22">
-        <v>0</v>
+      <c r="C103" s="17">
+        <v>47454.26</v>
       </c>
       <c r="D103" s="16"/>
-      <c r="E103" s="22">
-        <v>0</v>
+      <c r="E103" s="17">
+        <v>21504.18</v>
       </c>
       <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B104" s="16"/>
       <c r="C104" s="22">
@@ -2183,7 +2186,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B105" s="16"/>
       <c r="C105" s="22">
@@ -2197,7 +2200,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B106" s="16"/>
       <c r="C106" s="22">
@@ -2211,7 +2214,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B107" s="16"/>
       <c r="C107" s="22">
@@ -2223,40 +2226,46 @@
       </c>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" s="16"/>
+      <c r="C108" s="22">
+        <v>0</v>
+      </c>
+      <c r="D108" s="16"/>
+      <c r="E108" s="22">
+        <v>0</v>
+      </c>
+      <c r="F108" s="2"/>
+    </row>
+    <row r="109" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B108" s="16"/>
-      <c r="C108" s="23">
-        <v>0</v>
-      </c>
-      <c r="D108" s="21"/>
-      <c r="E108" s="23">
-        <v>0</v>
-      </c>
-      <c r="F108" s="2"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
+      <c r="B109" s="16"/>
+      <c r="C109" s="23">
+        <v>0</v>
+      </c>
+      <c r="D109" s="21"/>
+      <c r="E109" s="23">
+        <v>0</v>
+      </c>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B109" s="16"/>
-      <c r="C109" s="17">
-        <v>146912.94</v>
-      </c>
-      <c r="D109" s="16"/>
-      <c r="E109" s="17">
-        <v>92906.73</v>
-      </c>
-      <c r="F109" s="2"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="2"/>
       <c r="B110" s="16"/>
-      <c r="C110" s="16"/>
+      <c r="C110" s="17">
+        <v>124914.26</v>
+      </c>
       <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
+      <c r="E110" s="17">
+        <v>89129.18</v>
+      </c>
       <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2268,9 +2277,7 @@
       <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="A112" s="2"/>
       <c r="B112" s="16"/>
       <c r="C112" s="16"/>
       <c r="D112" s="16"/>
@@ -2278,26 +2285,22 @@
       <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
-        <v>36</v>
+      <c r="A113" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B113" s="16"/>
-      <c r="C113" s="17">
-        <v>104246.07</v>
-      </c>
+      <c r="C113" s="16"/>
       <c r="D113" s="16"/>
-      <c r="E113" s="22">
-        <v>0</v>
-      </c>
+      <c r="E113" s="16"/>
       <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="B114" s="16"/>
-      <c r="C114" s="22">
-        <v>0</v>
+      <c r="C114" s="17">
+        <v>40600</v>
       </c>
       <c r="D114" s="16"/>
       <c r="E114" s="22">
@@ -2307,35 +2310,35 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="B115" s="16"/>
       <c r="C115" s="22">
         <v>0</v>
       </c>
       <c r="D115" s="16"/>
-      <c r="E115" s="17">
-        <v>11702.02</v>
+      <c r="E115" s="22">
+        <v>0</v>
       </c>
       <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B116" s="16"/>
-      <c r="C116" s="22">
-        <v>0</v>
+      <c r="C116" s="17">
+        <v>9119.68</v>
       </c>
       <c r="D116" s="16"/>
-      <c r="E116" s="22">
-        <v>0</v>
+      <c r="E116" s="17">
+        <v>11323.29</v>
       </c>
       <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="B117" s="16"/>
       <c r="C117" s="22">
@@ -2349,7 +2352,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B118" s="16"/>
       <c r="C118" s="22">
@@ -2361,46 +2364,50 @@
       </c>
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B119" s="16"/>
+      <c r="C119" s="22">
+        <v>0</v>
+      </c>
+      <c r="D119" s="16"/>
+      <c r="E119" s="22">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2"/>
+    </row>
+    <row r="120" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B119" s="16"/>
-      <c r="C119" s="18">
-        <v>70000</v>
-      </c>
-      <c r="D119" s="21"/>
-      <c r="E119" s="23">
-        <v>0</v>
-      </c>
-      <c r="F119" s="2"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
+      <c r="B120" s="16"/>
+      <c r="C120" s="18">
+        <v>8440</v>
+      </c>
+      <c r="D120" s="21"/>
+      <c r="E120" s="23">
+        <v>0</v>
+      </c>
+      <c r="F120" s="2"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B120" s="2"/>
-      <c r="C120" s="17">
-        <v>174246.07</v>
-      </c>
-      <c r="D120" s="16"/>
-      <c r="E120" s="17">
-        <v>11702.02</v>
-      </c>
-      <c r="F120" s="2"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="2"/>
       <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
+      <c r="C121" s="17">
+        <v>58159.68</v>
+      </c>
+      <c r="D121" s="16"/>
+      <c r="E121" s="17">
+        <v>11323.29</v>
+      </c>
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="13" t="s">
-        <v>90</v>
-      </c>
+      <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -2408,73 +2415,73 @@
       <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
-        <v>91</v>
+      <c r="A123" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B123" s="2"/>
-      <c r="C123" s="7">
-        <v>0</v>
-      </c>
+      <c r="C123" s="2"/>
       <c r="D123" s="2"/>
-      <c r="E123" s="22">
-        <v>0</v>
-      </c>
+      <c r="E123" s="2"/>
       <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B124" s="2"/>
+      <c r="C124" s="7">
+        <v>0</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="22">
+        <v>0</v>
+      </c>
+      <c r="F124" s="2"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B124" s="16"/>
-      <c r="C124" s="7">
-        <v>0</v>
-      </c>
-      <c r="D124" s="16"/>
-      <c r="E124" s="22">
-        <v>0</v>
-      </c>
-      <c r="F124" s="2"/>
-    </row>
-    <row r="125" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="2" t="s">
+      <c r="B125" s="16"/>
+      <c r="C125" s="7">
+        <v>0</v>
+      </c>
+      <c r="D125" s="16"/>
+      <c r="E125" s="22">
+        <v>0</v>
+      </c>
+      <c r="F125" s="2"/>
+    </row>
+    <row r="126" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B125" s="16"/>
-      <c r="C125" s="20">
-        <v>0</v>
-      </c>
-      <c r="D125" s="21"/>
-      <c r="E125" s="23">
-        <v>0</v>
-      </c>
-      <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
+      <c r="B126" s="16"/>
+      <c r="C126" s="20">
+        <v>0</v>
+      </c>
+      <c r="D126" s="21"/>
+      <c r="E126" s="23">
+        <v>0</v>
+      </c>
+      <c r="F126" s="2"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B126" s="2"/>
-      <c r="C126" s="7">
-        <v>0</v>
-      </c>
-      <c r="D126" s="2"/>
-      <c r="E126" s="7">
-        <v>0</v>
-      </c>
-      <c r="F126" s="2"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="2"/>
       <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
+      <c r="C127" s="7">
+        <v>0</v>
+      </c>
       <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
+      <c r="E127" s="7">
+        <v>0</v>
+      </c>
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -2482,22 +2489,18 @@
       <c r="F128" s="2"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
-        <v>15</v>
+      <c r="A129" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="B129" s="2"/>
-      <c r="C129" s="7">
-        <v>0</v>
-      </c>
+      <c r="C129" s="2"/>
       <c r="D129" s="2"/>
-      <c r="E129" s="7">
-        <v>0</v>
-      </c>
+      <c r="E129" s="2"/>
       <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="7">
@@ -2509,46 +2512,50 @@
       </c>
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B131" s="2"/>
+      <c r="C131" s="7">
+        <v>0</v>
+      </c>
+      <c r="D131" s="2"/>
+      <c r="E131" s="7">
+        <v>0</v>
+      </c>
+      <c r="F131" s="2"/>
+    </row>
+    <row r="132" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B131" s="2"/>
-      <c r="C131" s="20">
-        <v>0</v>
-      </c>
-      <c r="D131" s="5"/>
-      <c r="E131" s="20">
-        <v>0</v>
-      </c>
-      <c r="F131" s="2"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
+      <c r="B132" s="2"/>
+      <c r="C132" s="20">
+        <v>0</v>
+      </c>
+      <c r="D132" s="5"/>
+      <c r="E132" s="20">
+        <v>0</v>
+      </c>
+      <c r="F132" s="2"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="7">
-        <v>0</v>
-      </c>
-      <c r="D132" s="2"/>
-      <c r="E132" s="7">
-        <v>0</v>
-      </c>
-      <c r="F132" s="2"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="2"/>
       <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
+      <c r="C133" s="7">
+        <v>0</v>
+      </c>
       <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
+      <c r="E133" s="7">
+        <v>0</v>
+      </c>
       <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="13" t="s">
-        <v>58</v>
-      </c>
+      <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -2556,53 +2563,55 @@
       <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
+      <c r="A135" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B135" s="2"/>
-      <c r="C135" s="7">
-        <v>0</v>
-      </c>
-      <c r="D135" s="2"/>
-      <c r="E135" s="7">
-        <v>0</v>
-      </c>
-      <c r="F135" s="2"/>
-    </row>
-    <row r="136" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="2" t="s">
+      <c r="B136" s="2"/>
+      <c r="C136" s="9">
+        <v>278191.59999999998</v>
+      </c>
+      <c r="D136" s="2"/>
+      <c r="E136" s="9">
+        <v>2070202.51</v>
+      </c>
+      <c r="F136" s="2"/>
+    </row>
+    <row r="137" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B136" s="2"/>
-      <c r="C136" s="20">
-        <v>0</v>
-      </c>
-      <c r="D136" s="5"/>
-      <c r="E136" s="14">
-        <v>2732.04</v>
-      </c>
-      <c r="F136" s="2"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
+      <c r="B137" s="2"/>
+      <c r="C137" s="14">
+        <v>15273.39</v>
+      </c>
+      <c r="D137" s="5"/>
+      <c r="E137" s="14">
+        <v>7751.88</v>
+      </c>
+      <c r="F137" s="2"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B137" s="2"/>
-      <c r="C137" s="7">
-        <v>0</v>
-      </c>
-      <c r="D137" s="2"/>
-      <c r="E137" s="9">
-        <v>2732.04</v>
-      </c>
-      <c r="F137" s="2"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="2"/>
       <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
+      <c r="C138" s="9">
+        <v>293464.99</v>
+      </c>
       <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
+      <c r="E138" s="9">
+        <v>2077954.39</v>
+      </c>
       <c r="F138" s="2"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -2614,9 +2623,7 @@
       <c r="F139" s="2"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A140" s="13" t="s">
-        <v>66</v>
-      </c>
+      <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -2624,22 +2631,18 @@
       <c r="F140" s="2"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
-        <v>95</v>
+      <c r="A141" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="B141" s="2"/>
-      <c r="C141" s="7">
-        <v>0</v>
-      </c>
+      <c r="C141" s="2"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="7">
-        <v>0</v>
-      </c>
+      <c r="E141" s="2"/>
       <c r="F141" s="2"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="7">
@@ -2653,21 +2656,21 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="7">
         <v>0</v>
       </c>
       <c r="D143" s="2"/>
-      <c r="E143" s="9">
-        <v>53000</v>
+      <c r="E143" s="7">
+        <v>0</v>
       </c>
       <c r="F143" s="2"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="7">
@@ -2681,7 +2684,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="7">
@@ -2695,7 +2698,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="7">
@@ -2709,9 +2712,9 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B147" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="B147" s="2"/>
       <c r="C147" s="7">
         <v>0</v>
       </c>
@@ -2723,7 +2726,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="B148" s="16"/>
       <c r="C148" s="7">
@@ -2737,9 +2740,9 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B149" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="B149" s="16"/>
       <c r="C149" s="7">
         <v>0</v>
       </c>
@@ -2751,159 +2754,159 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="7">
         <v>0</v>
       </c>
       <c r="D150" s="2"/>
-      <c r="E150" s="9">
-        <v>52000</v>
+      <c r="E150" s="7">
+        <v>0</v>
       </c>
       <c r="F150" s="2"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="7">
+        <v>0</v>
+      </c>
+      <c r="D151" s="2"/>
+      <c r="E151" s="9">
+        <v>269404</v>
+      </c>
+      <c r="F151" s="2"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="9">
-        <v>40000</v>
-      </c>
-      <c r="D151" s="2"/>
-      <c r="E151" s="7">
-        <v>0</v>
-      </c>
-      <c r="F151" s="2"/>
-    </row>
-    <row r="152" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="2" t="s">
+      <c r="B152" s="2"/>
+      <c r="C152" s="9">
+        <v>12255</v>
+      </c>
+      <c r="D152" s="2"/>
+      <c r="E152" s="7">
+        <v>0</v>
+      </c>
+      <c r="F152" s="2"/>
+    </row>
+    <row r="153" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="20">
-        <v>0</v>
-      </c>
-      <c r="D152" s="5"/>
-      <c r="E152" s="20">
-        <v>0</v>
-      </c>
-      <c r="F152" s="2"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" s="2" t="s">
+      <c r="B153" s="2"/>
+      <c r="C153" s="20">
+        <v>0</v>
+      </c>
+      <c r="D153" s="5"/>
+      <c r="E153" s="20">
+        <v>0</v>
+      </c>
+      <c r="F153" s="2"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B153" s="2"/>
-      <c r="C153" s="9">
-        <v>40000</v>
-      </c>
-      <c r="D153" s="2"/>
-      <c r="E153" s="9">
-        <v>105000</v>
-      </c>
-      <c r="F153" s="2"/>
-    </row>
-    <row r="154" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="2"/>
       <c r="B154" s="2"/>
-      <c r="C154" s="5"/>
-      <c r="D154" s="5"/>
-      <c r="E154" s="5"/>
+      <c r="C154" s="9">
+        <v>12255</v>
+      </c>
+      <c r="D154" s="2"/>
+      <c r="E154" s="9">
+        <v>269404</v>
+      </c>
       <c r="F154" s="2"/>
     </row>
     <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="3" t="s">
+      <c r="A155" s="2"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="2"/>
+    </row>
+    <row r="156" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B155" s="2"/>
-      <c r="C155" s="19">
-        <v>503099.01</v>
-      </c>
-      <c r="D155" s="5"/>
-      <c r="E155" s="19">
-        <v>597803.79</v>
-      </c>
-      <c r="F155" s="2"/>
-    </row>
-    <row r="156" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="2"/>
       <c r="B156" s="2"/>
-      <c r="C156" s="5"/>
+      <c r="C156" s="19">
+        <v>1194026.3799999999</v>
+      </c>
       <c r="D156" s="5"/>
-      <c r="E156" s="5"/>
+      <c r="E156" s="19">
+        <v>2800875.86</v>
+      </c>
       <c r="F156" s="2"/>
     </row>
-    <row r="157" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="3" t="s">
+    <row r="157" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="2"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="2"/>
+    </row>
+    <row r="158" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B157" s="2"/>
-      <c r="C157" s="19">
-        <v>664422.44999999995</v>
-      </c>
-      <c r="D157" s="5"/>
-      <c r="E157" s="19">
-        <v>1185407.28</v>
-      </c>
-      <c r="F157" s="2"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="2"/>
       <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="2"/>
+      <c r="C158" s="19">
+        <v>644352.01</v>
+      </c>
+      <c r="D158" s="5"/>
+      <c r="E158" s="19">
+        <v>436742.01</v>
+      </c>
       <c r="F158" s="2"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="2"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B159" s="24">
+      <c r="B160" s="24">
         <v>2023</v>
       </c>
-      <c r="C159" s="24"/>
-      <c r="D159" s="24">
+      <c r="C160" s="24"/>
+      <c r="D160" s="24">
         <v>2022</v>
       </c>
-      <c r="E159" s="24"/>
-      <c r="F159" s="10" t="s">
+      <c r="E160" s="24"/>
+      <c r="F160" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B160" s="2"/>
-      <c r="C160" s="7">
-        <v>0</v>
-      </c>
-      <c r="D160" s="2"/>
-      <c r="E160" s="9">
-        <v>1051175</v>
-      </c>
-      <c r="F160" s="2"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" s="7">
         <v>0</v>
       </c>
       <c r="D161" s="2"/>
-      <c r="E161" s="7">
-        <v>0</v>
+      <c r="E161" s="9">
+        <v>1322290</v>
       </c>
       <c r="F161" s="2"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="7">
@@ -2917,7 +2920,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="7">
@@ -2931,7 +2934,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" s="7">
@@ -2945,7 +2948,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="7">
@@ -2959,7 +2962,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" s="7">
@@ -2971,60 +2974,74 @@
       </c>
       <c r="F166" s="2"/>
     </row>
-    <row r="167" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B167" s="2"/>
+      <c r="C167" s="7">
+        <v>0</v>
+      </c>
+      <c r="D167" s="2"/>
+      <c r="E167" s="9">
+        <v>88000</v>
+      </c>
+      <c r="F167" s="2"/>
+    </row>
+    <row r="168" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B167" s="2"/>
-      <c r="C167" s="20">
-        <v>0</v>
-      </c>
-      <c r="D167" s="5"/>
-      <c r="E167" s="20">
-        <v>0</v>
-      </c>
-      <c r="F167" s="2"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A168" s="2" t="s">
+      <c r="B168" s="2"/>
+      <c r="C168" s="20">
+        <v>0</v>
+      </c>
+      <c r="D168" s="5"/>
+      <c r="E168" s="20">
+        <v>0</v>
+      </c>
+      <c r="F168" s="2"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B168" s="2"/>
-      <c r="C168" s="7">
-        <v>0</v>
-      </c>
-      <c r="D168" s="2"/>
-      <c r="E168" s="9">
-        <v>1051175</v>
-      </c>
-      <c r="F168" s="2"/>
-    </row>
-    <row r="169" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="2"/>
       <c r="B169" s="2"/>
-      <c r="C169" s="5"/>
-      <c r="D169" s="5"/>
-      <c r="E169" s="5"/>
+      <c r="C169" s="7">
+        <v>0</v>
+      </c>
+      <c r="D169" s="2"/>
+      <c r="E169" s="9">
+        <v>1410290</v>
+      </c>
       <c r="F169" s="2"/>
     </row>
-    <row r="170" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="3" t="s">
+    <row r="170" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="2"/>
+      <c r="B170" s="2"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="2"/>
+    </row>
+    <row r="171" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B170" s="2"/>
-      <c r="C170" s="19">
-        <v>664422.44999999995</v>
-      </c>
-      <c r="D170" s="5"/>
-      <c r="E170" s="19">
-        <v>134232.28</v>
-      </c>
-      <c r="F170" s="2"/>
+      <c r="B171" s="2"/>
+      <c r="C171" s="19">
+        <v>644352.01</v>
+      </c>
+      <c r="D171" s="5"/>
+      <c r="E171" s="19">
+        <v>-973547.99</v>
+      </c>
+      <c r="F171" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="D160:E160"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B63:C63"/>
@@ -3040,10 +3057,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E169"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:F170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3161,11 +3178,11 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="9">
-        <v>4977628.1100000003</v>
+        <v>5208628.24</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="9">
-        <v>4853594.49</v>
+        <v>6239461.1699999999</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -3189,11 +3206,11 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="14">
-        <v>900003.26</v>
+        <v>1050003.26</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="14">
-        <v>1500009.67</v>
+        <v>1670006.73</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -3203,11 +3220,11 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="9">
-        <v>5877631.3700000001</v>
+        <v>6258631.5</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="9">
-        <v>6353604.1600000001</v>
+        <v>7909467.9000000004</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -3235,7 +3252,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="9">
-        <v>832549.2</v>
+        <v>1529691.2</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="9">
@@ -3249,11 +3266,11 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="9">
-        <v>467764.08</v>
+        <v>443264.08</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="9">
-        <v>2059729.31</v>
+        <v>3298110.69</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -3291,11 +3308,11 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="9">
-        <v>517982.46</v>
+        <v>648468.02</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="9">
-        <v>280002.86</v>
+        <v>415002.95</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -3305,11 +3322,11 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="9">
-        <v>258401.08</v>
+        <v>169401.08</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="9">
-        <v>159000.13</v>
+        <v>169000.13</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -3333,11 +3350,11 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="9">
-        <v>2125446.8199999998</v>
+        <v>2839574.38</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="9">
-        <v>2682732.31</v>
+        <v>4066113.77</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -3373,11 +3390,11 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="9">
-        <v>675450.72</v>
+        <v>532150.72</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="9">
-        <v>294184.49</v>
+        <v>468536.82</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -3391,7 +3408,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="9">
-        <v>821525.3</v>
+        <v>874525.3</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -3443,11 +3460,11 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="9">
-        <v>802337.12</v>
+        <v>659037.12</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="9">
-        <v>1115709.79</v>
+        <v>1343062.13</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -3479,7 +3496,7 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="9">
-        <v>47810.7</v>
+        <v>102831.05</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -3521,7 +3538,7 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="9">
-        <v>47810.7</v>
+        <v>102831.05</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -3563,7 +3580,7 @@
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="14">
-        <v>1190.75</v>
+        <v>1441.45</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="14">
@@ -3577,7 +3594,7 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="9">
-        <v>1498651.6</v>
+        <v>1498902.3</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="9">
@@ -3637,7 +3654,7 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="9">
-        <v>18000</v>
+        <v>93500</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="9">
@@ -3665,11 +3682,11 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="9">
-        <v>28000</v>
+        <v>29000</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="9">
-        <v>10000</v>
+        <v>25999.99</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -3749,7 +3766,7 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="9">
-        <v>80000</v>
+        <v>72000</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="7">
@@ -3763,7 +3780,7 @@
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="14">
-        <v>41000</v>
+        <v>20000</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="20">
@@ -3777,11 +3794,11 @@
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="9">
-        <v>308549.84999999998</v>
+        <v>356049.85</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="9">
-        <v>32000</v>
+        <v>47999.99</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -3799,11 +3816,11 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="15">
-        <v>10612616.75</v>
+        <v>11612195.15</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="15">
-        <v>15645602.26</v>
+        <v>18883220.140000001</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -3855,11 +3872,11 @@
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="9">
-        <v>1990933.5</v>
+        <v>2265933.5</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="9">
-        <v>535000</v>
+        <v>758000</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -3869,11 +3886,11 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="9">
-        <v>221000</v>
+        <v>40000</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="9">
-        <v>313000</v>
+        <v>343000</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -3882,8 +3899,8 @@
         <v>77</v>
       </c>
       <c r="B67" s="2"/>
-      <c r="C67" s="9">
-        <v>50000</v>
+      <c r="C67" s="7">
+        <v>0</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="7">
@@ -3897,11 +3914,11 @@
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="14">
-        <v>80000</v>
+        <v>30000</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="14">
-        <v>16950</v>
+        <v>36950</v>
       </c>
       <c r="F68" s="2"/>
     </row>
@@ -3911,11 +3928,11 @@
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="9">
-        <v>2341933.5</v>
+        <v>2335933.5</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="9">
-        <v>864950</v>
+        <v>1137950</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -3933,7 +3950,7 @@
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="9">
-        <v>1243669.25</v>
+        <v>1041580.25</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="9">
@@ -3947,11 +3964,11 @@
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="9">
-        <v>164900</v>
+        <v>154900</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="9">
-        <v>100931.59</v>
+        <v>105931.59</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -3961,7 +3978,7 @@
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="14">
-        <v>100497.83</v>
+        <v>200022.28</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="20">
@@ -3975,11 +3992,11 @@
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="9">
-        <v>1509067.07</v>
+        <v>1396502.52</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="9">
-        <v>162046.59</v>
+        <v>167046.59</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -3997,7 +4014,7 @@
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="9">
-        <v>525550</v>
+        <v>495550</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="7">
@@ -4019,11 +4036,11 @@
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="9">
-        <v>3851000.57</v>
+        <v>3732436.02</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="9">
-        <v>1026996.59</v>
+        <v>1304996.5900000001</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -4171,7 +4188,7 @@
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="9">
-        <v>700614</v>
+        <v>719614</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="7">
@@ -4185,11 +4202,11 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="9">
-        <v>202479</v>
+        <v>260370</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="9">
-        <v>149688</v>
+        <v>224753</v>
       </c>
       <c r="F91" s="2"/>
     </row>
@@ -4199,7 +4216,7 @@
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="9">
-        <v>91824</v>
+        <v>178241</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="9">
@@ -4213,7 +4230,7 @@
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="9">
-        <v>72340.100000000006</v>
+        <v>143325.1</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="7">
@@ -4249,46 +4266,50 @@
       </c>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="7">
+        <v>0</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="7">
+        <v>0</v>
+      </c>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B96" s="2"/>
-      <c r="C96" s="20">
-        <v>0</v>
-      </c>
-      <c r="D96" s="5"/>
-      <c r="E96" s="20">
-        <v>0</v>
-      </c>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
+      <c r="B97" s="2"/>
+      <c r="C97" s="20">
+        <v>0</v>
+      </c>
+      <c r="D97" s="5"/>
+      <c r="E97" s="20">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="9">
-        <v>1915968.26</v>
-      </c>
-      <c r="D97" s="2"/>
-      <c r="E97" s="9">
-        <v>349718.87</v>
-      </c>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="2"/>
       <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
+      <c r="C98" s="9">
+        <v>2150261.2599999998</v>
+      </c>
       <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
+      <c r="E98" s="9">
+        <v>424783.87</v>
+      </c>
       <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -4296,54 +4317,50 @@
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B100" s="16"/>
-      <c r="C100" s="17">
-        <v>357620.32</v>
-      </c>
-      <c r="D100" s="16"/>
-      <c r="E100" s="17">
-        <v>448545</v>
-      </c>
+      <c r="A100" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B101" s="16"/>
       <c r="C101" s="17">
-        <v>282023.46999999997</v>
+        <v>435080.32</v>
       </c>
       <c r="D101" s="16"/>
       <c r="E101" s="17">
-        <v>131902.32</v>
+        <v>516170</v>
       </c>
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B102" s="16"/>
       <c r="C102" s="17">
-        <v>3425</v>
+        <v>329477.73</v>
       </c>
       <c r="D102" s="16"/>
-      <c r="E102" s="22">
-        <v>0</v>
+      <c r="E102" s="17">
+        <v>153406.5</v>
       </c>
       <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B103" s="16"/>
-      <c r="C103" s="22">
-        <v>0</v>
+      <c r="C103" s="17">
+        <v>3425</v>
       </c>
       <c r="D103" s="16"/>
       <c r="E103" s="22">
@@ -4353,7 +4370,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B104" s="16"/>
       <c r="C104" s="22">
@@ -4367,7 +4384,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B105" s="16"/>
       <c r="C105" s="22">
@@ -4381,7 +4398,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B106" s="16"/>
       <c r="C106" s="22">
@@ -4393,40 +4410,46 @@
       </c>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="16"/>
+      <c r="C107" s="22">
+        <v>0</v>
+      </c>
+      <c r="D107" s="16"/>
+      <c r="E107" s="22">
+        <v>0</v>
+      </c>
+      <c r="F107" s="2"/>
+    </row>
+    <row r="108" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B107" s="16"/>
-      <c r="C107" s="18">
+      <c r="B108" s="16"/>
+      <c r="C108" s="18">
         <v>291986</v>
       </c>
-      <c r="D107" s="21"/>
-      <c r="E107" s="18">
+      <c r="D108" s="21"/>
+      <c r="E108" s="18">
         <v>272513.64</v>
       </c>
-      <c r="F107" s="2"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
+      <c r="F108" s="2"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B108" s="16"/>
-      <c r="C108" s="17">
-        <v>935054.79</v>
-      </c>
-      <c r="D108" s="16"/>
-      <c r="E108" s="17">
-        <v>852960.96</v>
-      </c>
-      <c r="F108" s="2"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="2"/>
       <c r="B109" s="16"/>
-      <c r="C109" s="16"/>
+      <c r="C109" s="17">
+        <v>1059969.05</v>
+      </c>
       <c r="D109" s="16"/>
-      <c r="E109" s="16"/>
+      <c r="E109" s="17">
+        <v>942090.14</v>
+      </c>
       <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -4438,9 +4461,7 @@
       <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="A111" s="2"/>
       <c r="B111" s="16"/>
       <c r="C111" s="16"/>
       <c r="D111" s="16"/>
@@ -4448,82 +4469,78 @@
       <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>36</v>
+      <c r="A112" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B112" s="16"/>
-      <c r="C112" s="17">
-        <v>248790.56</v>
-      </c>
+      <c r="C112" s="16"/>
       <c r="D112" s="16"/>
-      <c r="E112" s="17">
-        <v>41285</v>
-      </c>
+      <c r="E112" s="16"/>
       <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="B113" s="16"/>
-      <c r="C113" s="22">
-        <v>0</v>
+      <c r="C113" s="17">
+        <v>255390.56</v>
       </c>
       <c r="D113" s="16"/>
-      <c r="E113" s="22">
-        <v>0</v>
+      <c r="E113" s="17">
+        <v>41285</v>
       </c>
       <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="B114" s="16"/>
-      <c r="C114" s="17">
-        <v>56244.85</v>
+      <c r="C114" s="22">
+        <v>0</v>
       </c>
       <c r="D114" s="16"/>
-      <c r="E114" s="17">
-        <v>67237.16</v>
+      <c r="E114" s="22">
+        <v>0</v>
       </c>
       <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B115" s="16"/>
-      <c r="C115" s="22">
-        <v>0</v>
+      <c r="C115" s="17">
+        <v>74526.37</v>
       </c>
       <c r="D115" s="16"/>
       <c r="E115" s="17">
-        <v>19458.099999999999</v>
+        <v>78560.45</v>
       </c>
       <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="B116" s="16"/>
       <c r="C116" s="22">
         <v>0</v>
       </c>
       <c r="D116" s="16"/>
-      <c r="E116" s="22">
-        <v>0</v>
+      <c r="E116" s="17">
+        <v>19458.099999999999</v>
       </c>
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B117" s="16"/>
-      <c r="C117" s="17">
-        <v>228455</v>
+      <c r="C117" s="22">
+        <v>0</v>
       </c>
       <c r="D117" s="16"/>
       <c r="E117" s="22">
@@ -4531,46 +4548,50 @@
       </c>
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B118" s="16"/>
+      <c r="C118" s="17">
+        <v>228455</v>
+      </c>
+      <c r="D118" s="16"/>
+      <c r="E118" s="22">
+        <v>0</v>
+      </c>
+      <c r="F118" s="2"/>
+    </row>
+    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B118" s="16"/>
-      <c r="C118" s="18">
-        <v>470616.67</v>
-      </c>
-      <c r="D118" s="21"/>
-      <c r="E118" s="18">
+      <c r="B119" s="16"/>
+      <c r="C119" s="18">
+        <v>409056.67</v>
+      </c>
+      <c r="D119" s="21"/>
+      <c r="E119" s="18">
         <v>263402.3</v>
       </c>
-      <c r="F118" s="2"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
+      <c r="F119" s="2"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B119" s="2"/>
-      <c r="C119" s="17">
-        <v>1004107.08</v>
-      </c>
-      <c r="D119" s="16"/>
-      <c r="E119" s="17">
-        <v>391382.56</v>
-      </c>
-      <c r="F119" s="2"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="2"/>
       <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
+      <c r="C120" s="17">
+        <v>967428.6</v>
+      </c>
+      <c r="D120" s="16"/>
+      <c r="E120" s="17">
+        <v>402705.85</v>
+      </c>
       <c r="F120" s="2"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="13" t="s">
-        <v>90</v>
-      </c>
+      <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -4578,73 +4599,73 @@
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
-        <v>91</v>
+      <c r="A122" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B122" s="2"/>
-      <c r="C122" s="7">
-        <v>0</v>
-      </c>
+      <c r="C122" s="2"/>
       <c r="D122" s="2"/>
-      <c r="E122" s="22">
-        <v>0</v>
-      </c>
+      <c r="E122" s="2"/>
       <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="7">
+        <v>0</v>
+      </c>
+      <c r="D123" s="2"/>
+      <c r="E123" s="22">
+        <v>0</v>
+      </c>
+      <c r="F123" s="2"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B123" s="16"/>
-      <c r="C123" s="7">
-        <v>0</v>
-      </c>
-      <c r="D123" s="16"/>
-      <c r="E123" s="22">
-        <v>0</v>
-      </c>
-      <c r="F123" s="2"/>
-    </row>
-    <row r="124" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="2" t="s">
+      <c r="B124" s="16"/>
+      <c r="C124" s="7">
+        <v>0</v>
+      </c>
+      <c r="D124" s="16"/>
+      <c r="E124" s="22">
+        <v>0</v>
+      </c>
+      <c r="F124" s="2"/>
+    </row>
+    <row r="125" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B124" s="16"/>
-      <c r="C124" s="20">
-        <v>0</v>
-      </c>
-      <c r="D124" s="21"/>
-      <c r="E124" s="23">
-        <v>0</v>
-      </c>
-      <c r="F124" s="2"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
+      <c r="B125" s="16"/>
+      <c r="C125" s="20">
+        <v>0</v>
+      </c>
+      <c r="D125" s="21"/>
+      <c r="E125" s="23">
+        <v>0</v>
+      </c>
+      <c r="F125" s="2"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B125" s="2"/>
-      <c r="C125" s="7">
-        <v>0</v>
-      </c>
-      <c r="D125" s="2"/>
-      <c r="E125" s="7">
-        <v>0</v>
-      </c>
-      <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="2"/>
       <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
+      <c r="C126" s="7">
+        <v>0</v>
+      </c>
       <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
+      <c r="E126" s="7">
+        <v>0</v>
+      </c>
       <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -4652,73 +4673,73 @@
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
-        <v>15</v>
+      <c r="A128" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="B128" s="2"/>
-      <c r="C128" s="7">
-        <v>0</v>
-      </c>
+      <c r="C128" s="2"/>
       <c r="D128" s="2"/>
-      <c r="E128" s="7">
-        <v>0</v>
-      </c>
+      <c r="E128" s="2"/>
       <c r="F128" s="2"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B129" s="2"/>
+      <c r="C129" s="7">
+        <v>0</v>
+      </c>
+      <c r="D129" s="2"/>
+      <c r="E129" s="7">
+        <v>0</v>
+      </c>
+      <c r="F129" s="2"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B129" s="2"/>
-      <c r="C129" s="9">
+      <c r="B130" s="2"/>
+      <c r="C130" s="9">
         <v>1391290</v>
       </c>
-      <c r="D129" s="2"/>
-      <c r="E129" s="9">
+      <c r="D130" s="2"/>
+      <c r="E130" s="9">
         <v>116290</v>
       </c>
-      <c r="F129" s="2"/>
-    </row>
-    <row r="130" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="2" t="s">
+      <c r="F130" s="2"/>
+    </row>
+    <row r="131" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B130" s="2"/>
-      <c r="C130" s="20">
-        <v>0</v>
-      </c>
-      <c r="D130" s="5"/>
-      <c r="E130" s="20">
-        <v>0</v>
-      </c>
-      <c r="F130" s="2"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
+      <c r="B131" s="2"/>
+      <c r="C131" s="20">
+        <v>0</v>
+      </c>
+      <c r="D131" s="5"/>
+      <c r="E131" s="20">
+        <v>0</v>
+      </c>
+      <c r="F131" s="2"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B131" s="2"/>
-      <c r="C131" s="9">
+      <c r="B132" s="2"/>
+      <c r="C132" s="9">
         <v>1391290</v>
       </c>
-      <c r="D131" s="2"/>
-      <c r="E131" s="9">
+      <c r="D132" s="2"/>
+      <c r="E132" s="9">
         <v>116290</v>
       </c>
-      <c r="F131" s="2"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
       <c r="F132" s="2"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="13" t="s">
-        <v>58</v>
-      </c>
+      <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
@@ -4726,53 +4747,55 @@
       <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B134" s="2"/>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B134" s="2"/>
-      <c r="C134" s="9">
-        <v>7456367.0999999996</v>
-      </c>
-      <c r="D134" s="2"/>
-      <c r="E134" s="9">
-        <v>427279.19</v>
-      </c>
-      <c r="F134" s="2"/>
-    </row>
-    <row r="135" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="2" t="s">
+      <c r="B135" s="2"/>
+      <c r="C135" s="9">
+        <v>7734558.7000000002</v>
+      </c>
+      <c r="D135" s="2"/>
+      <c r="E135" s="9">
+        <v>2497481.7000000002</v>
+      </c>
+      <c r="F135" s="2"/>
+    </row>
+    <row r="136" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B135" s="2"/>
-      <c r="C135" s="14">
-        <v>44146.13</v>
-      </c>
-      <c r="D135" s="5"/>
-      <c r="E135" s="14">
-        <v>27311.040000000001</v>
-      </c>
-      <c r="F135" s="2"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
+      <c r="B136" s="2"/>
+      <c r="C136" s="14">
+        <v>59419.519999999997</v>
+      </c>
+      <c r="D136" s="5"/>
+      <c r="E136" s="14">
+        <v>35062.92</v>
+      </c>
+      <c r="F136" s="2"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B136" s="2"/>
-      <c r="C136" s="9">
-        <v>7500513.2400000002</v>
-      </c>
-      <c r="D136" s="2"/>
-      <c r="E136" s="9">
-        <v>454590.23</v>
-      </c>
-      <c r="F136" s="2"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" s="2"/>
       <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
+      <c r="C137" s="9">
+        <v>7793978.2199999997</v>
+      </c>
       <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
+      <c r="E137" s="9">
+        <v>2532544.62</v>
+      </c>
       <c r="F137" s="2"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -4784,9 +4807,7 @@
       <c r="F138" s="2"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A139" s="13" t="s">
-        <v>66</v>
-      </c>
+      <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -4794,22 +4815,18 @@
       <c r="F139" s="2"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A140" s="2" t="s">
-        <v>95</v>
+      <c r="A140" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="B140" s="2"/>
-      <c r="C140" s="7">
-        <v>0</v>
-      </c>
+      <c r="C140" s="2"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="7">
-        <v>0</v>
-      </c>
+      <c r="E140" s="2"/>
       <c r="F140" s="2"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="7">
@@ -4823,65 +4840,65 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B142" s="2"/>
-      <c r="C142" s="9">
-        <v>90000</v>
+      <c r="C142" s="7">
+        <v>0</v>
       </c>
       <c r="D142" s="2"/>
-      <c r="E142" s="9">
-        <v>53000</v>
+      <c r="E142" s="7">
+        <v>0</v>
       </c>
       <c r="F142" s="2"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B143" s="2"/>
-      <c r="C143" s="7">
-        <v>0</v>
+      <c r="C143" s="9">
+        <v>90000</v>
       </c>
       <c r="D143" s="2"/>
-      <c r="E143" s="7">
-        <v>0</v>
+      <c r="E143" s="9">
+        <v>53000</v>
       </c>
       <c r="F143" s="2"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="7">
         <v>0</v>
       </c>
       <c r="D144" s="2"/>
-      <c r="E144" s="9">
-        <v>141524.41</v>
+      <c r="E144" s="7">
+        <v>0</v>
       </c>
       <c r="F144" s="2"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="7">
         <v>0</v>
       </c>
       <c r="D145" s="2"/>
-      <c r="E145" s="7">
-        <v>0</v>
+      <c r="E145" s="9">
+        <v>141524.41</v>
       </c>
       <c r="F145" s="2"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B146" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="B146" s="2"/>
       <c r="C146" s="7">
         <v>0</v>
       </c>
@@ -4893,11 +4910,11 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="B147" s="16"/>
-      <c r="C147" s="9">
-        <v>105030</v>
+      <c r="C147" s="7">
+        <v>0</v>
       </c>
       <c r="D147" s="2"/>
       <c r="E147" s="7">
@@ -4907,11 +4924,11 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B148" s="2"/>
-      <c r="C148" s="7">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="B148" s="16"/>
+      <c r="C148" s="9">
+        <v>105030</v>
       </c>
       <c r="D148" s="2"/>
       <c r="E148" s="7">
@@ -4919,189 +4936,189 @@
       </c>
       <c r="F148" s="2"/>
     </row>
-    <row r="149" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="7">
         <v>0</v>
       </c>
       <c r="D149" s="2"/>
-      <c r="E149" s="9">
-        <v>52000</v>
+      <c r="E149" s="7">
+        <v>0</v>
       </c>
       <c r="F149" s="2"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B150" s="2"/>
+      <c r="C150" s="7">
+        <v>0</v>
+      </c>
+      <c r="D150" s="2"/>
+      <c r="E150" s="9">
+        <v>321404</v>
+      </c>
+      <c r="F150" s="2"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B150" s="2"/>
-      <c r="C150" s="9">
-        <v>40000</v>
-      </c>
-      <c r="D150" s="2"/>
-      <c r="E150" s="7">
-        <v>0</v>
-      </c>
-      <c r="F150" s="2"/>
-    </row>
-    <row r="151" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="2" t="s">
+      <c r="B151" s="2"/>
+      <c r="C151" s="9">
+        <v>52255</v>
+      </c>
+      <c r="D151" s="2"/>
+      <c r="E151" s="7">
+        <v>0</v>
+      </c>
+      <c r="F151" s="2"/>
+    </row>
+    <row r="152" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="20">
-        <v>0</v>
-      </c>
-      <c r="D151" s="5"/>
-      <c r="E151" s="20">
-        <v>0</v>
-      </c>
-      <c r="F151" s="2"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" s="2" t="s">
+      <c r="B152" s="2"/>
+      <c r="C152" s="20">
+        <v>0</v>
+      </c>
+      <c r="D152" s="5"/>
+      <c r="E152" s="20">
+        <v>0</v>
+      </c>
+      <c r="F152" s="2"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="9">
-        <v>235030</v>
-      </c>
-      <c r="D152" s="2"/>
-      <c r="E152" s="9">
-        <v>246524.41</v>
-      </c>
-      <c r="F152" s="2"/>
-    </row>
-    <row r="153" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="2"/>
       <c r="B153" s="2"/>
-      <c r="C153" s="5"/>
-      <c r="D153" s="5"/>
-      <c r="E153" s="5"/>
+      <c r="C153" s="9">
+        <v>247285</v>
+      </c>
+      <c r="D153" s="2"/>
+      <c r="E153" s="9">
+        <v>515928.41</v>
+      </c>
       <c r="F153" s="2"/>
     </row>
     <row r="154" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="2"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="2"/>
+    </row>
+    <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B154" s="2"/>
-      <c r="C154" s="19">
-        <v>16832963.93</v>
-      </c>
-      <c r="D154" s="5"/>
-      <c r="E154" s="19">
-        <v>3438463.62</v>
-      </c>
-      <c r="F154" s="2"/>
-    </row>
-    <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="2"/>
       <c r="B155" s="2"/>
-      <c r="C155" s="5"/>
+      <c r="C155" s="19">
+        <v>17342648.149999999</v>
+      </c>
       <c r="D155" s="5"/>
-      <c r="E155" s="5"/>
+      <c r="E155" s="19">
+        <v>6239339.4900000002</v>
+      </c>
       <c r="F155" s="2"/>
     </row>
-    <row r="156" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="3" t="s">
+    <row r="156" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="2"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="2"/>
+    </row>
+    <row r="157" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B156" s="2"/>
-      <c r="C156" s="19">
-        <v>-6220347.1799999997</v>
-      </c>
-      <c r="D156" s="5"/>
-      <c r="E156" s="19">
-        <v>12207138.640000001</v>
-      </c>
-      <c r="F156" s="2"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="2"/>
       <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
-      <c r="E157" s="2"/>
+      <c r="C157" s="19">
+        <v>-5730453.0099999998</v>
+      </c>
+      <c r="D157" s="5"/>
+      <c r="E157" s="19">
+        <v>12643880.65</v>
+      </c>
       <c r="F157" s="2"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="2"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B158" s="24">
+      <c r="B159" s="24">
         <v>2023</v>
       </c>
-      <c r="C158" s="24"/>
-      <c r="D158" s="24">
+      <c r="C159" s="24"/>
+      <c r="D159" s="24">
         <v>2022</v>
       </c>
-      <c r="E158" s="24"/>
-      <c r="F158" s="10" t="s">
+      <c r="E159" s="24"/>
+      <c r="F159" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B159" s="2"/>
-      <c r="C159" s="7">
-        <v>0</v>
-      </c>
-      <c r="D159" s="2"/>
-      <c r="E159" s="9">
-        <v>1051175</v>
-      </c>
-      <c r="F159" s="2"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="7">
         <v>0</v>
       </c>
       <c r="D160" s="2"/>
-      <c r="E160" s="7">
-        <v>0</v>
+      <c r="E160" s="9">
+        <v>2373465</v>
       </c>
       <c r="F160" s="2"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="B161" s="2"/>
-      <c r="C161" s="9">
-        <v>134485</v>
+      <c r="C161" s="7">
+        <v>0</v>
       </c>
       <c r="D161" s="2"/>
-      <c r="E161" s="9">
-        <v>839367.31</v>
+      <c r="E161" s="7">
+        <v>0</v>
       </c>
       <c r="F161" s="2"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="B162" s="2"/>
-      <c r="C162" s="7">
-        <v>0</v>
+      <c r="C162" s="9">
+        <v>134485</v>
       </c>
       <c r="D162" s="2"/>
-      <c r="E162" s="7">
-        <v>0</v>
+      <c r="E162" s="9">
+        <v>839367.31</v>
       </c>
       <c r="F162" s="2"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="7">
@@ -5115,7 +5132,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" s="7">
@@ -5129,11 +5146,11 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B165" s="2"/>
-      <c r="C165" s="9">
-        <v>532851.89</v>
+      <c r="C165" s="7">
+        <v>0</v>
       </c>
       <c r="D165" s="2"/>
       <c r="E165" s="7">
@@ -5141,60 +5158,74 @@
       </c>
       <c r="F165" s="2"/>
     </row>
-    <row r="166" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B166" s="2"/>
+      <c r="C166" s="9">
+        <v>532851.89</v>
+      </c>
+      <c r="D166" s="2"/>
+      <c r="E166" s="9">
+        <v>88000</v>
+      </c>
+      <c r="F166" s="2"/>
+    </row>
+    <row r="167" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B166" s="2"/>
-      <c r="C166" s="20">
-        <v>0</v>
-      </c>
-      <c r="D166" s="5"/>
-      <c r="E166" s="14">
+      <c r="B167" s="2"/>
+      <c r="C167" s="20">
+        <v>0</v>
+      </c>
+      <c r="D167" s="5"/>
+      <c r="E167" s="14">
         <v>137036</v>
       </c>
-      <c r="F166" s="2"/>
-    </row>
-    <row r="167" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A167" s="2" t="s">
+      <c r="F167" s="2"/>
+    </row>
+    <row r="168" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B167" s="2"/>
-      <c r="C167" s="9">
+      <c r="B168" s="2"/>
+      <c r="C168" s="9">
         <v>667336.89</v>
       </c>
-      <c r="D167" s="2"/>
-      <c r="E167" s="9">
-        <v>2027578.31</v>
-      </c>
-      <c r="F167" s="2"/>
-    </row>
-    <row r="168" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="2"/>
-      <c r="B168" s="2"/>
-      <c r="C168" s="5"/>
-      <c r="D168" s="5"/>
-      <c r="E168" s="5"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="9">
+        <v>3437868.31</v>
+      </c>
       <c r="F168" s="2"/>
     </row>
-    <row r="169" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="3" t="s">
+    <row r="169" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="2"/>
+      <c r="B169" s="2"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="2"/>
+    </row>
+    <row r="170" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B169" s="2"/>
-      <c r="C169" s="19">
-        <v>-6887684.0700000003</v>
-      </c>
-      <c r="D169" s="5"/>
-      <c r="E169" s="19">
-        <v>10179560.32</v>
-      </c>
-      <c r="F169" s="2"/>
+      <c r="B170" s="2"/>
+      <c r="C170" s="19">
+        <v>-6397789.9000000004</v>
+      </c>
+      <c r="D170" s="5"/>
+      <c r="E170" s="19">
+        <v>9206012.3399999999</v>
+      </c>
+      <c r="F170" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="D159:E159"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B62:C62"/>

</xml_diff>

<commit_message>
Divisor para Plantinum Mediatraffic
</commit_message>
<xml_diff>
--- a/Copypega.xlsx
+++ b/Copypega.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\AppData\Local\Programs\Python\Python312\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFAEBA8-3C65-4232-BBCB-EF3E88315349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5ECE0E-1BAD-497A-B774-443F0021D1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="124">
   <si>
     <t>Ir al menu</t>
   </si>
@@ -399,7 +399,16 @@
     <t>Grupos de Estudio</t>
   </si>
   <si>
-    <t>Ala</t>
+    <t>Actividad de 50 aniversario</t>
+  </si>
+  <si>
+    <t>Actividad de Ordenacion de Bodhi</t>
+  </si>
+  <si>
+    <t>Atencion de visitantes - 50 aniversario/ordenacion</t>
+  </si>
+  <si>
+    <t>Menaje</t>
   </si>
 </sst>
 </file>
@@ -863,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:F171"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,11 +1005,11 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="9">
-        <v>283000.18</v>
+        <v>1234198.7</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="9">
-        <v>578864.64000000001</v>
+        <v>809420.88</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="9"/>
@@ -1028,8 +1037,8 @@
         <v>150000</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="20">
-        <v>0</v>
+      <c r="E13" s="14">
+        <v>389999.5</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1039,11 +1048,11 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="9">
-        <v>433000.18</v>
+        <v>1384198.7</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="9">
-        <v>578864.64000000001</v>
+        <v>1199420.3799999999</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1071,11 +1080,11 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="9">
-        <v>108822.3</v>
+        <v>473924.96</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="9">
-        <v>50000</v>
+      <c r="E17" s="7">
+        <v>0</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1088,8 +1097,8 @@
         <v>0</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="7">
-        <v>0</v>
+      <c r="E18" s="9">
+        <v>547800.34</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1098,12 +1107,12 @@
         <v>85</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="7">
-        <v>0</v>
+      <c r="C19" s="9">
+        <v>60000</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="7">
-        <v>0</v>
+      <c r="E19" s="9">
+        <v>118864</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1113,7 +1122,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="9">
-        <v>3000</v>
+        <v>73075</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="7">
@@ -1127,11 +1136,11 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="9">
-        <v>142636.26</v>
+        <v>210000</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="9">
-        <v>60000</v>
+        <v>47278.16</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1141,7 +1150,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="9">
-        <v>24000</v>
+        <v>4000</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="7">
@@ -1169,11 +1178,11 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="9">
-        <v>278458.56</v>
+        <v>820999.96</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="9">
-        <v>110000</v>
+        <v>713942.5</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -1209,11 +1218,11 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="9">
-        <v>10000</v>
+        <v>314006.12</v>
       </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="9">
-        <v>20000</v>
+      <c r="E28" s="7">
+        <v>0</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -1279,11 +1288,11 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="9">
-        <v>10000</v>
+        <v>314006.12</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="9">
-        <v>20000</v>
+      <c r="E33" s="7">
+        <v>0</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -1314,8 +1323,8 @@
         <v>0</v>
       </c>
       <c r="D36" s="2"/>
-      <c r="E36" s="9">
-        <v>158272.5</v>
+      <c r="E36" s="7">
+        <v>0</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -1356,8 +1365,8 @@
         <v>0</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="9">
-        <v>158272.5</v>
+      <c r="E39" s="7">
+        <v>0</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -1389,7 +1398,7 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="7">
-        <v>259.62</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -1398,12 +1407,12 @@
         <v>49</v>
       </c>
       <c r="B43" s="2"/>
-      <c r="C43" s="20">
-        <v>418.8</v>
+      <c r="C43" s="14">
+        <v>1600265.83</v>
       </c>
       <c r="D43" s="5"/>
-      <c r="E43" s="20">
-        <v>0</v>
+      <c r="E43" s="14">
+        <v>577432.23</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -1412,12 +1421,12 @@
         <v>48</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="7">
-        <v>418.8</v>
+      <c r="C44" s="9">
+        <v>1600265.83</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="7">
-        <v>259.62</v>
+      <c r="E44" s="9">
+        <v>577432.23</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -1472,8 +1481,8 @@
         <v>62</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="9">
-        <v>38500</v>
+      <c r="C49" s="7">
+        <v>0</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="7">
@@ -1486,8 +1495,8 @@
         <v>70</v>
       </c>
       <c r="B50" s="2"/>
-      <c r="C50" s="9">
-        <v>21000</v>
+      <c r="C50" s="7">
+        <v>0</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="7">
@@ -1500,8 +1509,8 @@
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="9">
-        <v>10000</v>
+      <c r="C51" s="7">
+        <v>0</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="7">
@@ -1612,8 +1621,8 @@
         <v>19</v>
       </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="9">
-        <v>69500</v>
+      <c r="C59" s="7">
+        <v>0</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="7">
@@ -1635,11 +1644,11 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="15">
-        <v>791377.54</v>
+        <v>4119470.61</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="15">
-        <v>867396.76</v>
+        <v>2490795.11</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -1691,11 +1700,11 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="9">
-        <v>400000</v>
+        <v>100000</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="9">
-        <v>150000</v>
+        <v>8000</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -1704,12 +1713,12 @@
         <v>24</v>
       </c>
       <c r="B67" s="2"/>
-      <c r="C67" s="7">
-        <v>0</v>
+      <c r="C67" s="9">
+        <v>55000</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="9">
-        <v>30000</v>
+        <v>16000</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -1736,8 +1745,8 @@
         <v>0</v>
       </c>
       <c r="D69" s="2"/>
-      <c r="E69" s="20">
-        <v>0</v>
+      <c r="E69" s="14">
+        <v>35000</v>
       </c>
       <c r="F69" s="2"/>
     </row>
@@ -1747,11 +1756,11 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="9">
-        <v>400000</v>
+        <v>155000</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="9">
-        <v>180000</v>
+        <v>59000</v>
       </c>
       <c r="F70" s="2"/>
     </row>
@@ -1769,11 +1778,11 @@
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="9">
-        <v>73225</v>
+        <v>29600</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="7">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -1811,11 +1820,11 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="9">
-        <v>73225</v>
+        <v>29600</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="7">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -1855,11 +1864,11 @@
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="9">
-        <v>473225</v>
+        <v>184600</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="9">
-        <v>180000</v>
+        <v>59675</v>
       </c>
       <c r="F79" s="2"/>
     </row>
@@ -1895,7 +1904,7 @@
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="9">
-        <v>313592</v>
+        <v>406020</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="7">
@@ -1908,8 +1917,8 @@
         <v>79</v>
       </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="9">
-        <v>19740</v>
+      <c r="C84" s="7">
+        <v>0</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="7">
@@ -1936,8 +1945,8 @@
         <v>101</v>
       </c>
       <c r="B86" s="2"/>
-      <c r="C86" s="7">
-        <v>0</v>
+      <c r="C86" s="9">
+        <v>342678.6</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="7">
@@ -1993,7 +2002,7 @@
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="9">
-        <v>333332</v>
+        <v>748698.6</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="7">
@@ -2006,8 +2015,8 @@
         <v>63</v>
       </c>
       <c r="B91" s="2"/>
-      <c r="C91" s="7">
-        <v>0</v>
+      <c r="C91" s="9">
+        <v>16750</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="7">
@@ -2020,8 +2029,8 @@
         <v>11</v>
       </c>
       <c r="B92" s="2"/>
-      <c r="C92" s="9">
-        <v>17107</v>
+      <c r="C92" s="7">
+        <v>0</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="7">
@@ -2034,8 +2043,8 @@
         <v>12</v>
       </c>
       <c r="B93" s="2"/>
-      <c r="C93" s="7">
-        <v>0</v>
+      <c r="C93" s="9">
+        <v>26525</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="7">
@@ -2066,8 +2075,8 @@
         <v>0</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="7">
-        <v>0</v>
+      <c r="E95" s="9">
+        <v>39000</v>
       </c>
       <c r="F95" s="2"/>
     </row>
@@ -2119,11 +2128,11 @@
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="9">
-        <v>350439</v>
+        <v>791973.6</v>
       </c>
       <c r="D99" s="2"/>
-      <c r="E99" s="7">
-        <v>0</v>
+      <c r="E99" s="9">
+        <v>39000</v>
       </c>
       <c r="F99" s="2"/>
     </row>
@@ -2151,11 +2160,11 @@
       </c>
       <c r="B102" s="16"/>
       <c r="C102" s="17">
-        <v>59180</v>
+        <v>59780</v>
       </c>
       <c r="D102" s="16"/>
       <c r="E102" s="17">
-        <v>70070</v>
+        <v>75135</v>
       </c>
       <c r="F102" s="2"/>
     </row>
@@ -2165,11 +2174,11 @@
       </c>
       <c r="B103" s="16"/>
       <c r="C103" s="17">
-        <v>47454.26</v>
+        <v>47465.15</v>
       </c>
       <c r="D103" s="16"/>
       <c r="E103" s="17">
-        <v>21401.94</v>
+        <v>21425.55</v>
       </c>
       <c r="F103" s="2"/>
     </row>
@@ -2252,8 +2261,8 @@
         <v>0</v>
       </c>
       <c r="D109" s="21"/>
-      <c r="E109" s="18">
-        <v>95423.62</v>
+      <c r="E109" s="23">
+        <v>0</v>
       </c>
       <c r="F109" s="2"/>
     </row>
@@ -2263,11 +2272,11 @@
       </c>
       <c r="B110" s="16"/>
       <c r="C110" s="17">
-        <v>106634.26</v>
+        <v>107245.15</v>
       </c>
       <c r="D110" s="16"/>
       <c r="E110" s="17">
-        <v>190130.56</v>
+        <v>99795.55</v>
       </c>
       <c r="F110" s="2"/>
     </row>
@@ -2306,8 +2315,8 @@
         <v>0</v>
       </c>
       <c r="D114" s="16"/>
-      <c r="E114" s="22">
-        <v>0</v>
+      <c r="E114" s="17">
+        <v>10000</v>
       </c>
       <c r="F114" s="2"/>
     </row>
@@ -2331,11 +2340,11 @@
       </c>
       <c r="B116" s="16"/>
       <c r="C116" s="17">
-        <v>9114.77</v>
+        <v>8787.18</v>
       </c>
       <c r="D116" s="16"/>
-      <c r="E116" s="17">
-        <v>10777.47</v>
+      <c r="E116" s="22">
+        <v>0</v>
       </c>
       <c r="F116" s="2"/>
     </row>
@@ -2391,7 +2400,7 @@
       </c>
       <c r="D120" s="21"/>
       <c r="E120" s="18">
-        <v>101830</v>
+        <v>59000</v>
       </c>
       <c r="F120" s="2"/>
     </row>
@@ -2401,11 +2410,11 @@
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="17">
-        <v>9114.77</v>
+        <v>8787.18</v>
       </c>
       <c r="D121" s="16"/>
       <c r="E121" s="17">
-        <v>112607.47</v>
+        <v>69000</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -2506,12 +2515,12 @@
         <v>15</v>
       </c>
       <c r="B130" s="2"/>
-      <c r="C130" s="7">
-        <v>0</v>
+      <c r="C130" s="9">
+        <v>199668.57</v>
       </c>
       <c r="D130" s="2"/>
-      <c r="E130" s="7">
-        <v>0</v>
+      <c r="E130" s="9">
+        <v>10000</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -2548,12 +2557,12 @@
         <v>53</v>
       </c>
       <c r="B133" s="2"/>
-      <c r="C133" s="7">
-        <v>0</v>
+      <c r="C133" s="9">
+        <v>199668.57</v>
       </c>
       <c r="D133" s="2"/>
-      <c r="E133" s="7">
-        <v>0</v>
+      <c r="E133" s="9">
+        <v>10000</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -2581,11 +2590,11 @@
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="9">
-        <v>859755.31</v>
+        <v>1038245.18</v>
       </c>
       <c r="D136" s="2"/>
       <c r="E136" s="9">
-        <v>2590750.2599999998</v>
+        <v>15430.07</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -2595,11 +2604,11 @@
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="14">
-        <v>6731.88</v>
+        <v>2329.23</v>
       </c>
       <c r="D137" s="5"/>
       <c r="E137" s="14">
-        <v>2591.2399999999998</v>
+        <v>86960.9</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -2609,11 +2618,11 @@
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="9">
-        <v>866487.19</v>
+        <v>1040574.41</v>
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="9">
-        <v>2593341.5</v>
+        <v>102390.97</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -2704,8 +2713,8 @@
         <v>50</v>
       </c>
       <c r="B146" s="2"/>
-      <c r="C146" s="9">
-        <v>44600</v>
+      <c r="C146" s="7">
+        <v>0</v>
       </c>
       <c r="D146" s="2"/>
       <c r="E146" s="7">
@@ -2774,8 +2783,8 @@
         <v>112</v>
       </c>
       <c r="B151" s="2"/>
-      <c r="C151" s="7">
-        <v>0</v>
+      <c r="C151" s="9">
+        <v>12000</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="7">
@@ -2817,7 +2826,7 @@
       </c>
       <c r="B154" s="2"/>
       <c r="C154" s="9">
-        <v>44600</v>
+        <v>12000</v>
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="7">
@@ -2839,11 +2848,11 @@
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="19">
-        <v>1850500.22</v>
+        <v>2344848.9</v>
       </c>
       <c r="D156" s="5"/>
       <c r="E156" s="19">
-        <v>3076079.53</v>
+        <v>379861.52</v>
       </c>
       <c r="F156" s="2"/>
     </row>
@@ -2861,11 +2870,11 @@
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="19">
-        <v>-1059122.68</v>
+        <v>1774621.7</v>
       </c>
       <c r="D158" s="5"/>
       <c r="E158" s="19">
-        <v>-2208682.77</v>
+        <v>2110933.59</v>
       </c>
       <c r="F158" s="2"/>
     </row>
@@ -2903,7 +2912,7 @@
       </c>
       <c r="D161" s="2"/>
       <c r="E161" s="9">
-        <v>1060001.1299999999</v>
+        <v>150000</v>
       </c>
       <c r="F161" s="2"/>
     </row>
@@ -3015,7 +3024,7 @@
       </c>
       <c r="D169" s="2"/>
       <c r="E169" s="9">
-        <v>1060001.1299999999</v>
+        <v>150000</v>
       </c>
       <c r="F169" s="2"/>
     </row>
@@ -3033,11 +3042,11 @@
       </c>
       <c r="B171" s="2"/>
       <c r="C171" s="19">
-        <v>-1059122.68</v>
+        <v>1774621.7</v>
       </c>
       <c r="D171" s="5"/>
       <c r="E171" s="19">
-        <v>-3268683.89</v>
+        <v>1960933.59</v>
       </c>
       <c r="F171" s="2"/>
     </row>
@@ -3060,10 +3069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F170"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3143,7 +3152,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="B7" s="24">
         <v>2023</v>
@@ -3181,11 +3190,11 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="9">
-        <v>5371628.4199999999</v>
+        <v>8470434.0199999996</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="9">
-        <v>6818325.8099999996</v>
+        <v>9377950.1899999995</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -3209,11 +3218,11 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="14">
-        <v>1200003.26</v>
+        <v>1800003.26</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="14">
-        <v>1670006.73</v>
+        <v>2600006.23</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -3223,11 +3232,11 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="9">
-        <v>6571631.6799999997</v>
+        <v>10270437.279999999</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="9">
-        <v>8488332.5399999991</v>
+        <v>11977956.42</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -3255,7 +3264,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="9">
-        <v>1638513.5</v>
+        <v>3874685.32</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="9">
@@ -3269,11 +3278,11 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="9">
-        <v>443264.08</v>
+        <v>467764.08</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="9">
-        <v>3298110.69</v>
+        <v>4651073.68</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -3282,12 +3291,12 @@
         <v>85</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="7">
-        <v>0</v>
+      <c r="C18" s="9">
+        <v>626127.19999999995</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="7">
-        <v>0</v>
+      <c r="E18" s="9">
+        <v>945410.5</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -3297,7 +3306,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="9">
-        <v>51750</v>
+        <v>128775</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="7">
@@ -3311,11 +3320,11 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="9">
-        <v>791104.28</v>
+        <v>1421104.28</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="9">
-        <v>475002.95</v>
+        <v>762275.35</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -3325,11 +3334,11 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="9">
-        <v>161401.07999999999</v>
+        <v>506401.08</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="9">
-        <v>169000.13</v>
+        <v>236000.11</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -3342,8 +3351,8 @@
         <v>0</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="20">
-        <v>0</v>
+      <c r="E22" s="14">
+        <v>48000</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -3353,11 +3362,11 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="9">
-        <v>3086032.94</v>
+        <v>7024856.96</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="9">
-        <v>4176113.77</v>
+        <v>6876759.6399999997</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -3393,11 +3402,11 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="9">
-        <v>530782.71999999997</v>
+        <v>1409416.64</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="9">
-        <v>488536.82</v>
+        <v>747977.82</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -3407,11 +3416,11 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="9">
-        <v>126886.39999999999</v>
+        <v>329425.56</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="9">
-        <v>874525.3</v>
+        <v>1532591.79</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -3420,8 +3429,8 @@
         <v>87</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="7">
-        <v>0</v>
+      <c r="C29" s="9">
+        <v>3000</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="7">
@@ -3443,170 +3452,170 @@
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="20">
-        <v>0</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="20">
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="7">
         <v>0</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="9">
-        <v>657669.12</v>
+      <c r="C32" s="7">
+        <v>0</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="9">
-        <v>1363062.13</v>
+      <c r="E32" s="7">
+        <v>0</v>
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
+    <row r="33" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="C33" s="7">
+        <v>0</v>
+      </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
-        <v>90</v>
+    <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="C34" s="7">
+        <v>0</v>
+      </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="E34" s="7">
+        <v>0</v>
+      </c>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>91</v>
-      </c>
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="7">
-        <v>0</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="9">
-        <v>261103.55</v>
-      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="9">
+        <v>1741842.19</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="9">
+        <v>2280569.61</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="7">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="9">
+        <v>261103.55</v>
+      </c>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="7">
-        <v>0</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="7">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="7">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="20">
-        <v>0</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="20">
-        <v>0</v>
-      </c>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="20">
+        <v>0</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="20">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="7">
-        <v>0</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="9">
+      <c r="B42" s="2"/>
+      <c r="C42" s="7">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="9">
         <v>261103.55</v>
       </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="9">
-        <v>1497460.85</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="9">
-        <v>5315699.68</v>
-      </c>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="14">
-        <v>1860.25</v>
-      </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="14">
-        <v>98305.24</v>
-      </c>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="9">
-        <v>1499321.1</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="9">
-        <v>5414004.9100000001</v>
-      </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -3614,144 +3623,138 @@
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="s">
-        <v>18</v>
+      <c r="A45" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="C45" s="9">
+        <v>1574223.26</v>
+      </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="E45" s="9">
+        <v>5315699.68</v>
+      </c>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="B46" s="2"/>
-      <c r="C46" s="7">
-        <v>0</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="7">
-        <v>0</v>
+      <c r="C46" s="14">
+        <v>1603340.43</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="14">
+        <v>675737.47</v>
       </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="9">
-        <v>58550</v>
+        <v>3177563.69</v>
       </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="7">
-        <v>0</v>
+      <c r="E47" s="9">
+        <v>5991437.1399999997</v>
       </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="9">
-        <v>132000</v>
-      </c>
+      <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="9">
-        <v>18000</v>
-      </c>
+      <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>70</v>
+      <c r="A49" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="9">
-        <v>103999.85</v>
-      </c>
+      <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="7">
-        <v>0</v>
-      </c>
+      <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="B50" s="2"/>
-      <c r="C50" s="9">
-        <v>39000</v>
+      <c r="C50" s="7">
+        <v>0</v>
       </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="9">
-        <v>25999.99</v>
+      <c r="E50" s="7">
+        <v>0</v>
       </c>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="7">
-        <v>0</v>
+      <c r="C51" s="9">
+        <v>64950</v>
       </c>
       <c r="D51" s="2"/>
-      <c r="E51" s="7">
-        <v>0</v>
+      <c r="E51" s="9">
+        <v>20005.98</v>
       </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="7">
-        <v>0</v>
+      <c r="C52" s="9">
+        <v>132000</v>
       </c>
       <c r="D52" s="2"/>
-      <c r="E52" s="7">
-        <v>0</v>
+      <c r="E52" s="9">
+        <v>54001.49</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="7">
-        <v>0</v>
+      <c r="C53" s="9">
+        <v>124999.85</v>
       </c>
       <c r="D53" s="2"/>
-      <c r="E53" s="9">
-        <v>4000</v>
+      <c r="E53" s="7">
+        <v>0</v>
       </c>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="B54" s="2"/>
-      <c r="C54" s="7">
-        <v>0</v>
+      <c r="C54" s="9">
+        <v>65000</v>
       </c>
       <c r="D54" s="2"/>
-      <c r="E54" s="7">
-        <v>0</v>
+      <c r="E54" s="9">
+        <v>25999.99</v>
       </c>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="7">
@@ -3765,11 +3768,11 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="9">
-        <v>72000</v>
+      <c r="C56" s="7">
+        <v>0</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="7">
@@ -3777,79 +3780,89 @@
       </c>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B57" s="2"/>
-      <c r="C57" s="14">
-        <v>20000</v>
-      </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="20">
-        <v>0</v>
+      <c r="C57" s="7">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="9">
+        <v>4000</v>
       </c>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="B58" s="2"/>
-      <c r="C58" s="9">
-        <v>425549.85</v>
+      <c r="C58" s="7">
+        <v>0</v>
       </c>
       <c r="D58" s="2"/>
-      <c r="E58" s="9">
-        <v>47999.99</v>
+      <c r="E58" s="7">
+        <v>0</v>
       </c>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="C59" s="7">
+        <v>0</v>
+      </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="E59" s="7">
+        <v>0</v>
+      </c>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="15">
-        <v>12240204.689999999</v>
+      <c r="C60" s="9">
+        <v>80000</v>
       </c>
       <c r="D60" s="2"/>
-      <c r="E60" s="15">
-        <v>19750616.890000001</v>
+      <c r="E60" s="7">
+        <v>0</v>
       </c>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="2"/>
+    <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="C61" s="14">
+        <v>41000</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="20">
+        <v>0</v>
+      </c>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62" s="24">
-        <v>2023</v>
-      </c>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24">
-        <v>2022</v>
-      </c>
-      <c r="E62" s="24"/>
-      <c r="F62" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="A62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="9">
+        <v>507949.85</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="9">
+        <v>104007.46</v>
+      </c>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
@@ -3860,190 +3873,192 @@
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="15">
+        <v>22722649.969999999</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="15">
+        <v>27491833.829999998</v>
+      </c>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="24">
+        <v>2023</v>
+      </c>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24">
+        <v>2022</v>
+      </c>
+      <c r="E66" s="24"/>
+      <c r="F66" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="9">
-        <v>2665933.5</v>
-      </c>
-      <c r="D65" s="2"/>
-      <c r="E65" s="9">
-        <v>908000</v>
-      </c>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="9">
-        <v>40000</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="9">
-        <v>373000</v>
-      </c>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="7">
-        <v>0</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="7">
-        <v>0</v>
-      </c>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="B68" s="2"/>
-      <c r="C68" s="20">
-        <v>0</v>
-      </c>
+      <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="14">
-        <v>36950</v>
-      </c>
+      <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="9">
-        <v>2705933.5</v>
+        <v>3327833.5</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="9">
-        <v>1317950</v>
+        <v>936000</v>
       </c>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="2"/>
+    <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="C70" s="9">
+        <v>621000</v>
+      </c>
       <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
+      <c r="E70" s="9">
+        <v>539000.14</v>
+      </c>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="9">
-        <v>1114805.25</v>
+        <v>50000</v>
       </c>
       <c r="D71" s="2"/>
-      <c r="E71" s="9">
-        <v>61115</v>
+      <c r="E71" s="7">
+        <v>0</v>
       </c>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="14">
+        <v>80000</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="14">
+        <v>71950</v>
+      </c>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="9">
+        <v>4078833.5</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="9">
+        <v>1546950.14</v>
+      </c>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="9">
+        <v>1788339.91</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="9">
+        <v>319214.5</v>
+      </c>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="9">
-        <v>154900</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="9">
-        <v>105931.59</v>
-      </c>
-      <c r="F72" s="2"/>
-    </row>
-    <row r="73" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="14">
-        <v>200022.28</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" s="20">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="9">
-        <v>1469727.52</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="9">
-        <v>167046.59</v>
-      </c>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="9">
-        <v>495550</v>
+        <v>291045</v>
       </c>
       <c r="D76" s="2"/>
-      <c r="E76" s="7">
-        <v>0</v>
+      <c r="E76" s="9">
+        <v>129707.02</v>
       </c>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="2"/>
+    <row r="77" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B77" s="2"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
+      <c r="C77" s="14">
+        <v>150252.65</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="14">
+        <v>35000</v>
+      </c>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="9">
-        <v>4175661.02</v>
+        <v>2229637.56</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="9">
-        <v>1484996.59</v>
+        <v>483921.52</v>
       </c>
       <c r="F78" s="2"/>
     </row>
@@ -4056,86 +4071,74 @@
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
+      <c r="A80" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="C80" s="9">
+        <v>565550</v>
+      </c>
       <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="E80" s="9">
+        <v>98122.2</v>
+      </c>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="13" t="s">
-        <v>44</v>
-      </c>
+    <row r="81" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="2"/>
       <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
       <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="9">
-        <v>892647.68</v>
+        <v>6308471.0599999996</v>
       </c>
       <c r="D82" s="2"/>
-      <c r="E82" s="7">
-        <v>0</v>
+      <c r="E82" s="9">
+        <v>2128993.85</v>
       </c>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
-        <v>79</v>
-      </c>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
       <c r="B83" s="2"/>
-      <c r="C83" s="9">
-        <v>127875</v>
-      </c>
+      <c r="C83" s="2"/>
       <c r="D83" s="2"/>
-      <c r="E83" s="7">
-        <v>0</v>
-      </c>
+      <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
-        <v>100</v>
-      </c>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="2"/>
       <c r="B84" s="2"/>
-      <c r="C84" s="7">
-        <v>0</v>
-      </c>
+      <c r="C84" s="2"/>
       <c r="D84" s="2"/>
-      <c r="E84" s="7">
-        <v>0</v>
-      </c>
+      <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>101</v>
+      <c r="A85" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B85" s="2"/>
-      <c r="C85" s="7">
-        <v>0</v>
-      </c>
+      <c r="C85" s="2"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="7">
-        <v>0</v>
-      </c>
+      <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B86" s="2"/>
-      <c r="C86" s="7">
-        <v>0</v>
+      <c r="C86" s="9">
+        <v>1861136.68</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="7">
@@ -4143,13 +4146,13 @@
       </c>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="9">
-        <v>16000</v>
+        <v>267277</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="7">
@@ -4157,27 +4160,27 @@
       </c>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B88" s="2"/>
-      <c r="C88" s="20">
-        <v>0</v>
-      </c>
-      <c r="D88" s="5"/>
-      <c r="E88" s="20">
+      <c r="C88" s="7">
+        <v>0</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="7">
         <v>0</v>
       </c>
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="9">
-        <v>1036522.68</v>
+        <v>749930.35</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="7">
@@ -4187,67 +4190,67 @@
     </row>
     <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="B90" s="2"/>
-      <c r="C90" s="9">
-        <v>719614</v>
+      <c r="C90" s="7">
+        <v>0</v>
       </c>
       <c r="D90" s="2"/>
-      <c r="E90" s="7">
-        <v>0</v>
+      <c r="E90" s="9">
+        <v>435659</v>
       </c>
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="9">
-        <v>277477</v>
+        <v>77500</v>
       </c>
       <c r="D91" s="2"/>
-      <c r="E91" s="9">
-        <v>224753</v>
+      <c r="E91" s="7">
+        <v>0</v>
       </c>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="B92" s="2"/>
-      <c r="C92" s="9">
-        <v>178241</v>
-      </c>
-      <c r="D92" s="2"/>
-      <c r="E92" s="9">
-        <v>160900</v>
+      <c r="C92" s="20">
+        <v>0</v>
+      </c>
+      <c r="D92" s="5"/>
+      <c r="E92" s="20">
+        <v>0</v>
       </c>
       <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="9">
-        <v>143325.1</v>
+        <v>2955844.03</v>
       </c>
       <c r="D93" s="2"/>
-      <c r="E93" s="7">
-        <v>0</v>
+      <c r="E93" s="9">
+        <v>435659</v>
       </c>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="B94" s="2"/>
-      <c r="C94" s="7">
-        <v>0</v>
+      <c r="C94" s="9">
+        <v>745864</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="7">
@@ -4257,380 +4260,390 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="9">
-        <v>145520.48000000001</v>
+        <v>561265</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="9">
-        <v>39130.870000000003</v>
+        <v>302085</v>
       </c>
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="7">
-        <v>0</v>
+      <c r="C96" s="9">
+        <v>299471.34999999998</v>
       </c>
       <c r="D96" s="2"/>
-      <c r="E96" s="7">
-        <v>0</v>
+      <c r="E96" s="9">
+        <v>240172</v>
       </c>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B97" s="2"/>
-      <c r="C97" s="20">
-        <v>0</v>
-      </c>
-      <c r="D97" s="5"/>
-      <c r="E97" s="20">
+      <c r="C97" s="9">
+        <v>157105.1</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="7">
         <v>0</v>
       </c>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="B98" s="2"/>
-      <c r="C98" s="9">
-        <v>2500700.2599999998</v>
+      <c r="C98" s="7">
+        <v>0</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="9">
-        <v>424783.87</v>
+        <v>194916</v>
       </c>
       <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="2"/>
+      <c r="A99" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
+      <c r="C99" s="9">
+        <v>283099.37</v>
+      </c>
       <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
+      <c r="E99" s="9">
+        <v>109115.08</v>
+      </c>
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="13" t="s">
-        <v>30</v>
+      <c r="A100" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
+      <c r="C100" s="7">
+        <v>0</v>
+      </c>
       <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
+      <c r="E100" s="7">
+        <v>0</v>
+      </c>
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B101" s="16"/>
-      <c r="C101" s="17">
-        <v>494260.32</v>
-      </c>
-      <c r="D101" s="16"/>
-      <c r="E101" s="17">
-        <v>586240</v>
+        <v>120</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="C101" s="7">
+        <v>0</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="7">
+        <v>0</v>
       </c>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B102" s="16"/>
-      <c r="C102" s="17">
-        <v>376931.99</v>
-      </c>
-      <c r="D102" s="16"/>
-      <c r="E102" s="17">
-        <v>174808.44</v>
+        <v>121</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="7">
+        <v>0</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="7">
+        <v>0</v>
       </c>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B103" s="16"/>
-      <c r="C103" s="17">
-        <v>3425</v>
-      </c>
-      <c r="D103" s="16"/>
-      <c r="E103" s="17">
-        <v>3235</v>
+        <v>122</v>
+      </c>
+      <c r="B103" s="2"/>
+      <c r="C103" s="7">
+        <v>0</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="7">
+        <v>0</v>
       </c>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B104" s="16"/>
-      <c r="C104" s="22">
-        <v>0</v>
-      </c>
-      <c r="D104" s="16"/>
-      <c r="E104" s="22">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B104" s="2"/>
+      <c r="C104" s="14">
+        <v>58906</v>
+      </c>
+      <c r="D104" s="5"/>
+      <c r="E104" s="14">
+        <v>120792</v>
       </c>
       <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B105" s="16"/>
-      <c r="C105" s="22">
-        <v>0</v>
-      </c>
-      <c r="D105" s="16"/>
-      <c r="E105" s="22">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="B105" s="2"/>
+      <c r="C105" s="9">
+        <v>5061554.8499999996</v>
+      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" s="9">
+        <v>1402739.08</v>
       </c>
       <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B106" s="16"/>
-      <c r="C106" s="22">
-        <v>0</v>
-      </c>
-      <c r="D106" s="16"/>
-      <c r="E106" s="22">
-        <v>0</v>
-      </c>
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
       <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B107" s="16"/>
-      <c r="C107" s="22">
-        <v>0</v>
-      </c>
-      <c r="D107" s="16"/>
-      <c r="E107" s="22">
-        <v>0</v>
-      </c>
+      <c r="A107" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B108" s="16"/>
-      <c r="C108" s="18">
-        <v>291986</v>
-      </c>
-      <c r="D108" s="21"/>
-      <c r="E108" s="18">
-        <v>367937.26</v>
+      <c r="C108" s="17">
+        <v>789610.32</v>
+      </c>
+      <c r="D108" s="16"/>
+      <c r="E108" s="17">
+        <v>895550</v>
       </c>
       <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B109" s="16"/>
       <c r="C109" s="17">
-        <v>1166603.31</v>
+        <v>566894.79</v>
       </c>
       <c r="D109" s="16"/>
       <c r="E109" s="17">
-        <v>1132220.7</v>
+        <v>261964.01</v>
       </c>
       <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="2"/>
+      <c r="A110" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="B110" s="16"/>
-      <c r="C110" s="16"/>
+      <c r="C110" s="17">
+        <v>3425</v>
+      </c>
       <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
+      <c r="E110" s="17">
+        <v>6470</v>
+      </c>
       <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="2"/>
+      <c r="A111" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B111" s="16"/>
-      <c r="C111" s="16"/>
+      <c r="C111" s="22">
+        <v>0</v>
+      </c>
       <c r="D111" s="16"/>
-      <c r="E111" s="16"/>
+      <c r="E111" s="22">
+        <v>0</v>
+      </c>
       <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="13" t="s">
-        <v>35</v>
+      <c r="A112" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B112" s="16"/>
-      <c r="C112" s="16"/>
+      <c r="C112" s="22">
+        <v>0</v>
+      </c>
       <c r="D112" s="16"/>
-      <c r="E112" s="16"/>
+      <c r="E112" s="22">
+        <v>0</v>
+      </c>
       <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="B113" s="16"/>
       <c r="C113" s="17">
-        <v>255390.56</v>
+        <v>633076.16</v>
       </c>
       <c r="D113" s="16"/>
       <c r="E113" s="17">
-        <v>41285</v>
+        <v>734801.59</v>
       </c>
       <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B114" s="16"/>
-      <c r="C114" s="22">
-        <v>0</v>
+      <c r="C114" s="17">
+        <v>60220</v>
       </c>
       <c r="D114" s="16"/>
-      <c r="E114" s="22">
-        <v>0</v>
+      <c r="E114" s="17">
+        <v>65111.77</v>
       </c>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B115" s="16"/>
-      <c r="C115" s="17">
-        <v>83641.14</v>
-      </c>
-      <c r="D115" s="16"/>
-      <c r="E115" s="17">
-        <v>89337.919999999998</v>
+      <c r="C115" s="18">
+        <v>485132.36</v>
+      </c>
+      <c r="D115" s="21"/>
+      <c r="E115" s="18">
+        <v>367937.26</v>
       </c>
       <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B116" s="16"/>
-      <c r="C116" s="22">
-        <v>0</v>
+      <c r="C116" s="17">
+        <v>2538358.63</v>
       </c>
       <c r="D116" s="16"/>
       <c r="E116" s="17">
-        <v>19458.099999999999</v>
+        <v>2331834.63</v>
       </c>
       <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="A117" s="2"/>
       <c r="B117" s="16"/>
-      <c r="C117" s="22">
-        <v>0</v>
-      </c>
+      <c r="C117" s="16"/>
       <c r="D117" s="16"/>
-      <c r="E117" s="22">
-        <v>0</v>
-      </c>
+      <c r="E117" s="16"/>
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="1:6" ht="27" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>74</v>
-      </c>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="2"/>
       <c r="B118" s="16"/>
-      <c r="C118" s="17">
-        <v>228455</v>
-      </c>
+      <c r="C118" s="16"/>
       <c r="D118" s="16"/>
-      <c r="E118" s="22">
-        <v>0</v>
-      </c>
+      <c r="E118" s="16"/>
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="2" t="s">
-        <v>38</v>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B119" s="16"/>
-      <c r="C119" s="18">
-        <v>409056.67</v>
-      </c>
-      <c r="D119" s="21"/>
-      <c r="E119" s="18">
-        <v>365232.3</v>
-      </c>
+      <c r="C119" s="16"/>
+      <c r="D119" s="16"/>
+      <c r="E119" s="16"/>
       <c r="F119" s="2"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B120" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B120" s="16"/>
       <c r="C120" s="17">
-        <v>976543.38</v>
+        <v>309390.56</v>
       </c>
       <c r="D120" s="16"/>
       <c r="E120" s="17">
-        <v>515313.32</v>
+        <v>116482.65</v>
       </c>
       <c r="F120" s="2"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
+      <c r="A121" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B121" s="16"/>
+      <c r="C121" s="22">
+        <v>0</v>
+      </c>
+      <c r="D121" s="16"/>
+      <c r="E121" s="22">
+        <v>0</v>
+      </c>
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
+      <c r="A122" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B122" s="16"/>
+      <c r="C122" s="17">
+        <v>119387.31</v>
+      </c>
+      <c r="D122" s="16"/>
+      <c r="E122" s="17">
+        <v>120953.17</v>
+      </c>
       <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B123" s="2"/>
-      <c r="C123" s="7">
-        <v>0</v>
-      </c>
-      <c r="D123" s="2"/>
-      <c r="E123" s="22">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="B123" s="16"/>
+      <c r="C123" s="22">
+        <v>0</v>
+      </c>
+      <c r="D123" s="16"/>
+      <c r="E123" s="17">
+        <v>19458.099999999999</v>
       </c>
       <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B124" s="16"/>
-      <c r="C124" s="7">
+      <c r="C124" s="22">
         <v>0</v>
       </c>
       <c r="D124" s="16"/>
@@ -4639,46 +4652,50 @@
       </c>
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B125" s="16"/>
-      <c r="C125" s="20">
-        <v>0</v>
-      </c>
-      <c r="D125" s="21"/>
-      <c r="E125" s="23">
+      <c r="C125" s="17">
+        <v>228455</v>
+      </c>
+      <c r="D125" s="16"/>
+      <c r="E125" s="22">
         <v>0</v>
       </c>
       <c r="F125" s="2"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B126" s="2"/>
-      <c r="C126" s="7">
-        <v>0</v>
-      </c>
-      <c r="D126" s="2"/>
-      <c r="E126" s="7">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="B126" s="16"/>
+      <c r="C126" s="18">
+        <v>512504.67</v>
+      </c>
+      <c r="D126" s="21"/>
+      <c r="E126" s="18">
+        <v>521017.3</v>
       </c>
       <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="2"/>
+      <c r="A127" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
+      <c r="C127" s="17">
+        <v>1169737.55</v>
+      </c>
+      <c r="D127" s="16"/>
+      <c r="E127" s="17">
+        <v>777911.22</v>
+      </c>
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -4686,73 +4703,73 @@
       <c r="F128" s="2"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
-        <v>15</v>
+      <c r="A129" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B129" s="2"/>
-      <c r="C129" s="7">
-        <v>0</v>
-      </c>
+      <c r="C129" s="2"/>
       <c r="D129" s="2"/>
-      <c r="E129" s="7">
-        <v>0</v>
-      </c>
+      <c r="E129" s="2"/>
       <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B130" s="2"/>
-      <c r="C130" s="9">
-        <v>1391290</v>
+      <c r="C130" s="7">
+        <v>0</v>
       </c>
       <c r="D130" s="2"/>
-      <c r="E130" s="9">
-        <v>116290</v>
+      <c r="E130" s="22">
+        <v>0</v>
       </c>
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B131" s="2"/>
-      <c r="C131" s="20">
-        <v>0</v>
-      </c>
-      <c r="D131" s="5"/>
-      <c r="E131" s="20">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="B131" s="16"/>
+      <c r="C131" s="7">
+        <v>0</v>
+      </c>
+      <c r="D131" s="16"/>
+      <c r="E131" s="17">
+        <v>42448</v>
       </c>
       <c r="F131" s="2"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B132" s="16"/>
+      <c r="C132" s="20">
+        <v>0</v>
+      </c>
+      <c r="D132" s="21"/>
+      <c r="E132" s="23">
+        <v>0</v>
+      </c>
+      <c r="F132" s="2"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="9">
-        <v>1391290</v>
-      </c>
-      <c r="D132" s="2"/>
-      <c r="E132" s="9">
-        <v>116290</v>
-      </c>
-      <c r="F132" s="2"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="2"/>
       <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
+      <c r="C133" s="7">
+        <v>0</v>
+      </c>
       <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
+      <c r="E133" s="9">
+        <v>42448</v>
+      </c>
       <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="13" t="s">
-        <v>58</v>
-      </c>
+      <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -4760,67 +4777,73 @@
       <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
-        <v>46</v>
+      <c r="A135" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="B135" s="2"/>
-      <c r="C135" s="9">
-        <v>8594314.0099999998</v>
-      </c>
+      <c r="C135" s="2"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="9">
-        <v>5088231.96</v>
-      </c>
+      <c r="E135" s="2"/>
       <c r="F135" s="2"/>
     </row>
-    <row r="136" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B136" s="2"/>
-      <c r="C136" s="14">
-        <v>66151.399999999994</v>
-      </c>
-      <c r="D136" s="5"/>
-      <c r="E136" s="14">
-        <v>37654.160000000003</v>
+      <c r="C136" s="9">
+        <v>260668.57</v>
+      </c>
+      <c r="D136" s="2"/>
+      <c r="E136" s="9">
+        <v>10000</v>
       </c>
       <c r="F136" s="2"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="9">
-        <v>8660465.4100000001</v>
+        <v>1391290</v>
       </c>
       <c r="D137" s="2"/>
       <c r="E137" s="9">
-        <v>5125886.12</v>
+        <v>116290</v>
       </c>
       <c r="F137" s="2"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="2"/>
+    <row r="138" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
+      <c r="C138" s="14">
+        <v>126000</v>
+      </c>
+      <c r="D138" s="5"/>
+      <c r="E138" s="20">
+        <v>0</v>
+      </c>
       <c r="F138" s="2"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A139" s="2"/>
+      <c r="A139" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
+      <c r="C139" s="9">
+        <v>1777958.57</v>
+      </c>
       <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
+      <c r="E139" s="9">
+        <v>126290</v>
+      </c>
       <c r="F139" s="2"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A140" s="13" t="s">
-        <v>66</v>
-      </c>
+      <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -4828,110 +4851,90 @@
       <c r="F140" s="2"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
-        <v>95</v>
+      <c r="A141" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="B141" s="2"/>
-      <c r="C141" s="7">
-        <v>0</v>
-      </c>
+      <c r="C141" s="2"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="7">
-        <v>0</v>
-      </c>
+      <c r="E141" s="2"/>
       <c r="F141" s="2"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B142" s="2"/>
-      <c r="C142" s="7">
-        <v>0</v>
+      <c r="C142" s="9">
+        <v>10347234.630000001</v>
       </c>
       <c r="D142" s="2"/>
-      <c r="E142" s="7">
-        <v>0</v>
+      <c r="E142" s="9">
+        <v>11285493.619999999</v>
       </c>
       <c r="F142" s="2"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B143" s="2"/>
-      <c r="C143" s="9">
-        <v>90000</v>
-      </c>
-      <c r="D143" s="2"/>
-      <c r="E143" s="9">
-        <v>53000</v>
+      <c r="C143" s="14">
+        <v>105050.37</v>
+      </c>
+      <c r="D143" s="5"/>
+      <c r="E143" s="14">
+        <v>135628.34</v>
       </c>
       <c r="F143" s="2"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B144" s="2"/>
-      <c r="C144" s="7">
-        <v>0</v>
+      <c r="C144" s="9">
+        <v>10452285</v>
       </c>
       <c r="D144" s="2"/>
-      <c r="E144" s="7">
-        <v>0</v>
+      <c r="E144" s="9">
+        <v>11421121.970000001</v>
       </c>
       <c r="F144" s="2"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="A145" s="2"/>
       <c r="B145" s="2"/>
-      <c r="C145" s="9">
-        <v>44600</v>
-      </c>
+      <c r="C145" s="2"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="9">
-        <v>141524.41</v>
-      </c>
+      <c r="E145" s="2"/>
       <c r="F145" s="2"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A146" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="A146" s="2"/>
       <c r="B146" s="2"/>
-      <c r="C146" s="7">
-        <v>0</v>
-      </c>
+      <c r="C146" s="2"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="7">
-        <v>0</v>
-      </c>
+      <c r="E146" s="2"/>
       <c r="F146" s="2"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B147" s="16"/>
-      <c r="C147" s="7">
-        <v>0</v>
-      </c>
+      <c r="A147" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="7">
-        <v>0</v>
-      </c>
+      <c r="E147" s="2"/>
       <c r="F147" s="2"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B148" s="16"/>
-      <c r="C148" s="9">
-        <v>105030</v>
+        <v>95</v>
+      </c>
+      <c r="B148" s="2"/>
+      <c r="C148" s="7">
+        <v>0</v>
       </c>
       <c r="D148" s="2"/>
       <c r="E148" s="7">
@@ -4941,39 +4944,39 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="7">
         <v>0</v>
       </c>
       <c r="D149" s="2"/>
-      <c r="E149" s="7">
-        <v>0</v>
+      <c r="E149" s="9">
+        <v>41036</v>
       </c>
       <c r="F149" s="2"/>
     </row>
-    <row r="150" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="B150" s="2"/>
-      <c r="C150" s="7">
-        <v>0</v>
+      <c r="C150" s="9">
+        <v>90000</v>
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="9">
-        <v>321404</v>
+        <v>53000</v>
       </c>
       <c r="F150" s="2"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B151" s="2"/>
-      <c r="C151" s="9">
-        <v>52255</v>
+      <c r="C151" s="7">
+        <v>0</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="7">
@@ -4981,258 +4984,370 @@
       </c>
       <c r="F151" s="2"/>
     </row>
-    <row r="152" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="B152" s="2"/>
-      <c r="C152" s="20">
-        <v>0</v>
-      </c>
-      <c r="D152" s="5"/>
-      <c r="E152" s="20">
+      <c r="C152" s="7">
+        <v>0</v>
+      </c>
+      <c r="D152" s="2"/>
+      <c r="E152" s="7">
         <v>0</v>
       </c>
       <c r="F152" s="2"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="9">
-        <v>291885</v>
+        <v>68160</v>
       </c>
       <c r="D153" s="2"/>
       <c r="E153" s="9">
-        <v>515928.41</v>
+        <v>141524.41</v>
       </c>
       <c r="F153" s="2"/>
     </row>
-    <row r="154" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="2"/>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="B154" s="2"/>
-      <c r="C154" s="5"/>
-      <c r="D154" s="5"/>
-      <c r="E154" s="5"/>
+      <c r="C154" s="7">
+        <v>0</v>
+      </c>
+      <c r="D154" s="2"/>
+      <c r="E154" s="7">
+        <v>0</v>
+      </c>
       <c r="F154" s="2"/>
     </row>
-    <row r="155" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B155" s="2"/>
-      <c r="C155" s="19">
-        <v>19163148.379999999</v>
-      </c>
-      <c r="D155" s="5"/>
-      <c r="E155" s="19">
-        <v>9315419.0099999998</v>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B155" s="16"/>
+      <c r="C155" s="7">
+        <v>0</v>
+      </c>
+      <c r="D155" s="2"/>
+      <c r="E155" s="7">
+        <v>0</v>
       </c>
       <c r="F155" s="2"/>
     </row>
-    <row r="156" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="2"/>
-      <c r="B156" s="2"/>
-      <c r="C156" s="5"/>
-      <c r="D156" s="5"/>
-      <c r="E156" s="5"/>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B156" s="16"/>
+      <c r="C156" s="9">
+        <v>105030</v>
+      </c>
+      <c r="D156" s="2"/>
+      <c r="E156" s="7">
+        <v>0</v>
+      </c>
       <c r="F156" s="2"/>
     </row>
-    <row r="157" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="3" t="s">
-        <v>43</v>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B157" s="2"/>
-      <c r="C157" s="19">
-        <v>-6922943.6900000004</v>
-      </c>
-      <c r="D157" s="5"/>
-      <c r="E157" s="19">
-        <v>10435197.880000001</v>
+      <c r="C157" s="7">
+        <v>0</v>
+      </c>
+      <c r="D157" s="2"/>
+      <c r="E157" s="7">
+        <v>0</v>
       </c>
       <c r="F157" s="2"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="2"/>
+    <row r="158" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A158" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
+      <c r="C158" s="9">
+        <v>12000</v>
+      </c>
       <c r="D158" s="2"/>
-      <c r="E158" s="2"/>
+      <c r="E158" s="9">
+        <v>373924.8</v>
+      </c>
       <c r="F158" s="2"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B159" s="24">
-        <v>2023</v>
-      </c>
-      <c r="C159" s="24"/>
-      <c r="D159" s="24">
-        <v>2022</v>
-      </c>
-      <c r="E159" s="24"/>
-      <c r="F159" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B159" s="2"/>
+      <c r="C159" s="9">
+        <v>52255</v>
+      </c>
+      <c r="D159" s="2"/>
+      <c r="E159" s="7">
+        <v>0</v>
+      </c>
+      <c r="F159" s="2"/>
+    </row>
+    <row r="160" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="B160" s="2"/>
-      <c r="C160" s="7">
-        <v>0</v>
-      </c>
-      <c r="D160" s="2"/>
-      <c r="E160" s="9">
-        <v>3433466.13</v>
+      <c r="C160" s="20">
+        <v>0</v>
+      </c>
+      <c r="D160" s="5"/>
+      <c r="E160" s="20">
+        <v>0</v>
       </c>
       <c r="F160" s="2"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="B161" s="2"/>
-      <c r="C161" s="7">
-        <v>0</v>
+      <c r="C161" s="9">
+        <v>327445</v>
       </c>
       <c r="D161" s="2"/>
-      <c r="E161" s="7">
-        <v>0</v>
+      <c r="E161" s="9">
+        <v>609485.21</v>
       </c>
       <c r="F161" s="2"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
-        <v>41</v>
-      </c>
+    <row r="162" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="2"/>
       <c r="B162" s="2"/>
-      <c r="C162" s="9">
-        <v>134485</v>
-      </c>
-      <c r="D162" s="2"/>
-      <c r="E162" s="9">
-        <v>839367.31</v>
-      </c>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="5"/>
       <c r="F162" s="2"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
-        <v>115</v>
+    <row r="163" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B163" s="2"/>
-      <c r="C163" s="7">
-        <v>0</v>
-      </c>
-      <c r="D163" s="2"/>
-      <c r="E163" s="7">
-        <v>0</v>
+      <c r="C163" s="19">
+        <v>27635810.649999999</v>
+      </c>
+      <c r="D163" s="5"/>
+      <c r="E163" s="19">
+        <v>18840823.969999999</v>
       </c>
       <c r="F163" s="2"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A164" s="2" t="s">
-        <v>116</v>
-      </c>
+    <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="2"/>
       <c r="B164" s="2"/>
-      <c r="C164" s="7">
-        <v>0</v>
-      </c>
-      <c r="D164" s="2"/>
-      <c r="E164" s="7">
-        <v>0</v>
-      </c>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5"/>
       <c r="F164" s="2"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
-        <v>117</v>
+    <row r="165" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B165" s="2"/>
-      <c r="C165" s="7">
-        <v>0</v>
-      </c>
-      <c r="D165" s="2"/>
-      <c r="E165" s="7">
-        <v>0</v>
+      <c r="C165" s="19">
+        <v>-4913160.67</v>
+      </c>
+      <c r="D165" s="5"/>
+      <c r="E165" s="19">
+        <v>8651009.8599999994</v>
       </c>
       <c r="F165" s="2"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A166" s="2" t="s">
-        <v>118</v>
-      </c>
+      <c r="A166" s="2"/>
       <c r="B166" s="2"/>
-      <c r="C166" s="9">
-        <v>532851.89</v>
-      </c>
+      <c r="C166" s="2"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="9">
-        <v>88000</v>
-      </c>
+      <c r="E166" s="2"/>
       <c r="F166" s="2"/>
     </row>
-    <row r="167" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B167" s="2"/>
-      <c r="C167" s="20">
-        <v>0</v>
-      </c>
-      <c r="D167" s="5"/>
-      <c r="E167" s="14">
-        <v>137036</v>
-      </c>
-      <c r="F167" s="2"/>
-    </row>
-    <row r="168" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B167" s="24">
+        <v>2023</v>
+      </c>
+      <c r="C167" s="24"/>
+      <c r="D167" s="24">
+        <v>2022</v>
+      </c>
+      <c r="E167" s="24"/>
+      <c r="F167" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" s="9">
-        <v>667336.89</v>
+        <v>425000</v>
       </c>
       <c r="D168" s="2"/>
       <c r="E168" s="9">
-        <v>4497869.4400000004</v>
+        <v>5344619.04</v>
       </c>
       <c r="F168" s="2"/>
     </row>
-    <row r="169" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="2"/>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B169" s="2"/>
-      <c r="C169" s="5"/>
-      <c r="D169" s="5"/>
-      <c r="E169" s="5"/>
+      <c r="C169" s="7">
+        <v>0</v>
+      </c>
+      <c r="D169" s="2"/>
+      <c r="E169" s="7">
+        <v>0</v>
+      </c>
       <c r="F169" s="2"/>
     </row>
-    <row r="170" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="3" t="s">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B170" s="2"/>
+      <c r="C170" s="9">
+        <v>134485</v>
+      </c>
+      <c r="D170" s="2"/>
+      <c r="E170" s="9">
+        <v>839367.31</v>
+      </c>
+      <c r="F170" s="2"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B171" s="2"/>
+      <c r="C171" s="7">
+        <v>0</v>
+      </c>
+      <c r="D171" s="2"/>
+      <c r="E171" s="7">
+        <v>0</v>
+      </c>
+      <c r="F171" s="2"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B172" s="2"/>
+      <c r="C172" s="7">
+        <v>0</v>
+      </c>
+      <c r="D172" s="2"/>
+      <c r="E172" s="7">
+        <v>0</v>
+      </c>
+      <c r="F172" s="2"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B173" s="2"/>
+      <c r="C173" s="7">
+        <v>0</v>
+      </c>
+      <c r="D173" s="2"/>
+      <c r="E173" s="7">
+        <v>0</v>
+      </c>
+      <c r="F173" s="2"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B174" s="2"/>
+      <c r="C174" s="9">
+        <v>532851.89</v>
+      </c>
+      <c r="D174" s="2"/>
+      <c r="E174" s="9">
+        <v>88000</v>
+      </c>
+      <c r="F174" s="2"/>
+    </row>
+    <row r="175" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B175" s="2"/>
+      <c r="C175" s="14">
+        <v>396277.5</v>
+      </c>
+      <c r="D175" s="5"/>
+      <c r="E175" s="14">
+        <v>179976</v>
+      </c>
+      <c r="F175" s="2"/>
+    </row>
+    <row r="176" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A176" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B176" s="2"/>
+      <c r="C176" s="9">
+        <v>1488614.39</v>
+      </c>
+      <c r="D176" s="2"/>
+      <c r="E176" s="9">
+        <v>6451962.3499999996</v>
+      </c>
+      <c r="F176" s="2"/>
+    </row>
+    <row r="177" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A177" s="2"/>
+      <c r="B177" s="2"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="2"/>
+    </row>
+    <row r="178" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A178" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B170" s="2"/>
-      <c r="C170" s="19">
-        <v>-7590280.5800000001</v>
-      </c>
-      <c r="D170" s="5"/>
-      <c r="E170" s="19">
-        <v>5937328.4400000004</v>
-      </c>
-      <c r="F170" s="2"/>
+      <c r="B178" s="2"/>
+      <c r="C178" s="19">
+        <v>-6401775.0700000003</v>
+      </c>
+      <c r="D178" s="5"/>
+      <c r="E178" s="19">
+        <v>2199047.5099999998</v>
+      </c>
+      <c r="F178" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="D167:E167"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="gid=1453964497" display="gid=1453964497" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>